<commit_message>
[Pipette] 1/5 work update
</commit_message>
<xml_diff>
--- a/Plasma Project schedule V1.0.xlsx
+++ b/Plasma Project schedule V1.0.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A74973-42FE-4087-B491-71E2D2E46447}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="20181224" sheetId="20" r:id="rId1"/>
@@ -14,17 +13,17 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'20181224'!$A$1:$A$30</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>만든 이</author>
   </authors>
   <commentList>
-    <comment ref="Y7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="Y7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -39,7 +38,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="AH7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="AN7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -69,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DM7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="DM7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="DT7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="DT7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -99,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="FC7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="FC7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Femto Project 일정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -178,10 +177,6 @@
   </si>
   <si>
     <t>◇ MP1 Sample 입고 : 4ea</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>◇ F/W debugging</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -311,11 +306,33 @@
     <t>RF Generator 회로 및 PCB 작업</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>◇ F/W debugging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>◇ Trans case 입고 2ea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>◇ battery 입고 4ea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>◇ 1Set 전달</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Pipette case 입고.
+Pipette 1set 전달.
+조립 후 Test </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1081,7 +1098,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1245,6 +1262,62 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1287,36 +1360,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1326,35 +1369,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1400,7 +1418,7 @@
         <xdr:cNvPr id="52" name="직선 화살표 연결선 51">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1457,7 +1475,7 @@
         <xdr:cNvPr id="15" name="직선 화살표 연결선 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1498,23 +1516,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>122</xdr:col>
-      <xdr:colOff>156882</xdr:colOff>
+      <xdr:col>135</xdr:col>
+      <xdr:colOff>224117</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>68481</xdr:rowOff>
+      <xdr:rowOff>124511</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>128</xdr:col>
-      <xdr:colOff>161365</xdr:colOff>
+      <xdr:col>140</xdr:col>
+      <xdr:colOff>127747</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>68481</xdr:rowOff>
+      <xdr:rowOff>124511</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="18" name="직선 화살표 연결선 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B9B7B3B-4B32-4051-898C-EE6F25736D05}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B9B7B3B-4B32-4051-898C-EE6F25736D05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1522,8 +1540,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="25051870" y="2345516"/>
-          <a:ext cx="1187824" cy="0"/>
+          <a:off x="36531176" y="2399305"/>
+          <a:ext cx="1360395" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1555,23 +1573,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>126</xdr:col>
-      <xdr:colOff>85165</xdr:colOff>
+      <xdr:col>137</xdr:col>
+      <xdr:colOff>275665</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>77445</xdr:rowOff>
+      <xdr:rowOff>111063</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>133</xdr:col>
-      <xdr:colOff>161365</xdr:colOff>
+      <xdr:col>143</xdr:col>
+      <xdr:colOff>172572</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>77445</xdr:rowOff>
+      <xdr:rowOff>111063</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="21" name="직선 화살표 연결선 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEEB29C9-2143-40DD-9242-A82E285F4B2E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEEB29C9-2143-40DD-9242-A82E285F4B2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1579,8 +1597,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="25769047" y="2524810"/>
-          <a:ext cx="1456765" cy="0"/>
+          <a:off x="37165430" y="2587563"/>
+          <a:ext cx="1645024" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1612,23 +1630,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>142</xdr:col>
-      <xdr:colOff>192741</xdr:colOff>
+      <xdr:col>154</xdr:col>
+      <xdr:colOff>203947</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>95375</xdr:rowOff>
+      <xdr:rowOff>117786</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>177</xdr:col>
-      <xdr:colOff>179294</xdr:colOff>
+      <xdr:col>193</xdr:col>
+      <xdr:colOff>11207</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>95375</xdr:rowOff>
+      <xdr:rowOff>117786</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="25" name="직선 화살표 연결선 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2375196F-31DF-4BFC-AC62-19AF714F443A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2375196F-31DF-4BFC-AC62-19AF714F443A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1636,8 +1654,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29032200" y="2713069"/>
-          <a:ext cx="6889376" cy="0"/>
+          <a:off x="42046712" y="2795992"/>
+          <a:ext cx="9477936" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1685,7 +1703,7 @@
         <xdr:cNvPr id="28" name="직선 화살표 연결선 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D1266C4-6D7E-4F8B-8103-59BF7C6FE4FB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D1266C4-6D7E-4F8B-8103-59BF7C6FE4FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1742,7 +1760,7 @@
         <xdr:cNvPr id="32" name="직선 화살표 연결선 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{666CF52C-5D68-4474-8BDD-79976E036787}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{666CF52C-5D68-4474-8BDD-79976E036787}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1799,7 +1817,7 @@
         <xdr:cNvPr id="33" name="직선 화살표 연결선 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07D67EB1-AD43-42F4-B443-3BB978B9F2AC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07D67EB1-AD43-42F4-B443-3BB978B9F2AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1856,7 +1874,7 @@
         <xdr:cNvPr id="36" name="직선 화살표 연결선 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A732A08-4D4F-441D-9243-033ACD4A7F32}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A732A08-4D4F-441D-9243-033ACD4A7F32}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1913,7 +1931,7 @@
         <xdr:cNvPr id="38" name="직선 화살표 연결선 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A864090-2577-47BA-8983-FFA17538A224}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A864090-2577-47BA-8983-FFA17538A224}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1970,7 +1988,7 @@
         <xdr:cNvPr id="41" name="직선 화살표 연결선 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B9CC53C-2611-4F5F-B122-A3165CFAFB90}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B9CC53C-2611-4F5F-B122-A3165CFAFB90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2027,7 +2045,7 @@
         <xdr:cNvPr id="46" name="직선 화살표 연결선 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6CC6FD7-49CF-4859-9978-820DB474FDCC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6CC6FD7-49CF-4859-9978-820DB474FDCC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2084,7 +2102,7 @@
         <xdr:cNvPr id="14" name="직선 화살표 연결선 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5A7DBF8-E685-466C-85D3-36D1828C9CBD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5A7DBF8-E685-466C-85D3-36D1828C9CBD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2141,7 +2159,7 @@
         <xdr:cNvPr id="16" name="직선 화살표 연결선 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D724AD7-DEC3-4BAD-A0BE-EBB685097DA0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D724AD7-DEC3-4BAD-A0BE-EBB685097DA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2198,7 +2216,7 @@
         <xdr:cNvPr id="19" name="직선 화살표 연결선 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E49A8F08-60DF-418D-8D92-E435C42894A7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E49A8F08-60DF-418D-8D92-E435C42894A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2283,7 +2301,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2316,26 +2334,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2368,23 +2369,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2560,352 +2544,352 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:JN47"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CI1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DN36" sqref="DN36"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AU1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BG18" sqref="BG18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.59765625" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.3984375" style="52" customWidth="1"/>
-    <col min="2" max="10" width="2.69921875" style="55" bestFit="1" customWidth="1"/>
-    <col min="11" max="31" width="3.69921875" style="55" bestFit="1" customWidth="1"/>
-    <col min="32" max="40" width="2.69921875" style="55" bestFit="1" customWidth="1"/>
-    <col min="41" max="62" width="3.69921875" style="55" bestFit="1" customWidth="1"/>
-    <col min="63" max="71" width="2.69921875" style="55" bestFit="1" customWidth="1"/>
-    <col min="72" max="92" width="3.69921875" style="55" bestFit="1" customWidth="1"/>
-    <col min="93" max="101" width="2.69921875" style="55" bestFit="1" customWidth="1"/>
-    <col min="102" max="123" width="3.69921875" style="55" bestFit="1" customWidth="1"/>
-    <col min="124" max="132" width="2.69921875" style="55" bestFit="1" customWidth="1"/>
-    <col min="133" max="154" width="3.69921875" style="55" bestFit="1" customWidth="1"/>
-    <col min="155" max="163" width="2.69921875" style="55" bestFit="1" customWidth="1"/>
-    <col min="164" max="182" width="3.69921875" style="55" bestFit="1" customWidth="1"/>
-    <col min="183" max="16384" width="2.59765625" style="55"/>
+    <col min="1" max="1" width="10.375" style="52" customWidth="1"/>
+    <col min="2" max="10" width="2.75" style="55" bestFit="1" customWidth="1"/>
+    <col min="11" max="31" width="3.75" style="55" bestFit="1" customWidth="1"/>
+    <col min="32" max="40" width="2.75" style="55" bestFit="1" customWidth="1"/>
+    <col min="41" max="62" width="3.75" style="55" bestFit="1" customWidth="1"/>
+    <col min="63" max="71" width="2.75" style="55" bestFit="1" customWidth="1"/>
+    <col min="72" max="92" width="3.75" style="55" bestFit="1" customWidth="1"/>
+    <col min="93" max="101" width="2.75" style="55" bestFit="1" customWidth="1"/>
+    <col min="102" max="123" width="3.75" style="55" bestFit="1" customWidth="1"/>
+    <col min="124" max="132" width="2.75" style="55" bestFit="1" customWidth="1"/>
+    <col min="133" max="154" width="3.75" style="55" bestFit="1" customWidth="1"/>
+    <col min="155" max="163" width="2.75" style="55" bestFit="1" customWidth="1"/>
+    <col min="164" max="182" width="3.75" style="55" bestFit="1" customWidth="1"/>
+    <col min="183" max="16384" width="2.625" style="55"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:274" s="54" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:274" s="54" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:274" s="54" customFormat="1" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:274" s="54" customFormat="1" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="48" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:274" s="54" customFormat="1" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:274" s="54" customFormat="1" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="48" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:274" s="54" customFormat="1" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:274" s="54" customFormat="1" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="49" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:274" s="54" customFormat="1" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:274" s="54" customFormat="1" ht="17.25" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="50" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:274" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:274" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="51"/>
-      <c r="B6" s="142">
+      <c r="B6" s="162">
         <v>9</v>
       </c>
-      <c r="C6" s="143"/>
-      <c r="D6" s="143"/>
-      <c r="E6" s="143"/>
-      <c r="F6" s="143"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="143"/>
-      <c r="I6" s="143"/>
-      <c r="J6" s="143"/>
-      <c r="K6" s="143"/>
-      <c r="L6" s="143"/>
-      <c r="M6" s="143"/>
-      <c r="N6" s="143"/>
-      <c r="O6" s="143"/>
-      <c r="P6" s="143"/>
-      <c r="Q6" s="143"/>
-      <c r="R6" s="143"/>
-      <c r="S6" s="143"/>
-      <c r="T6" s="143"/>
-      <c r="U6" s="143"/>
-      <c r="V6" s="143"/>
-      <c r="W6" s="143"/>
-      <c r="X6" s="143"/>
-      <c r="Y6" s="143"/>
-      <c r="Z6" s="143"/>
-      <c r="AA6" s="143"/>
-      <c r="AB6" s="143"/>
-      <c r="AC6" s="143"/>
-      <c r="AD6" s="143"/>
-      <c r="AE6" s="144"/>
-      <c r="AF6" s="139">
+      <c r="C6" s="163"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="163"/>
+      <c r="G6" s="163"/>
+      <c r="H6" s="163"/>
+      <c r="I6" s="163"/>
+      <c r="J6" s="163"/>
+      <c r="K6" s="163"/>
+      <c r="L6" s="163"/>
+      <c r="M6" s="163"/>
+      <c r="N6" s="163"/>
+      <c r="O6" s="163"/>
+      <c r="P6" s="163"/>
+      <c r="Q6" s="163"/>
+      <c r="R6" s="163"/>
+      <c r="S6" s="163"/>
+      <c r="T6" s="163"/>
+      <c r="U6" s="163"/>
+      <c r="V6" s="163"/>
+      <c r="W6" s="163"/>
+      <c r="X6" s="163"/>
+      <c r="Y6" s="163"/>
+      <c r="Z6" s="163"/>
+      <c r="AA6" s="163"/>
+      <c r="AB6" s="163"/>
+      <c r="AC6" s="163"/>
+      <c r="AD6" s="163"/>
+      <c r="AE6" s="164"/>
+      <c r="AF6" s="159">
         <v>10</v>
       </c>
-      <c r="AG6" s="139"/>
-      <c r="AH6" s="139"/>
-      <c r="AI6" s="139"/>
-      <c r="AJ6" s="139"/>
-      <c r="AK6" s="139"/>
-      <c r="AL6" s="139"/>
-      <c r="AM6" s="139"/>
-      <c r="AN6" s="139"/>
-      <c r="AO6" s="139"/>
-      <c r="AP6" s="139"/>
-      <c r="AQ6" s="139"/>
-      <c r="AR6" s="139"/>
-      <c r="AS6" s="139"/>
-      <c r="AT6" s="139"/>
-      <c r="AU6" s="139"/>
-      <c r="AV6" s="139"/>
-      <c r="AW6" s="139"/>
-      <c r="AX6" s="139"/>
-      <c r="AY6" s="139"/>
-      <c r="AZ6" s="139"/>
-      <c r="BA6" s="139"/>
-      <c r="BB6" s="139"/>
-      <c r="BC6" s="139"/>
-      <c r="BD6" s="139"/>
-      <c r="BE6" s="139"/>
-      <c r="BF6" s="139"/>
-      <c r="BG6" s="139"/>
-      <c r="BH6" s="139"/>
-      <c r="BI6" s="139"/>
-      <c r="BJ6" s="140"/>
-      <c r="BK6" s="142">
+      <c r="AG6" s="159"/>
+      <c r="AH6" s="159"/>
+      <c r="AI6" s="159"/>
+      <c r="AJ6" s="159"/>
+      <c r="AK6" s="159"/>
+      <c r="AL6" s="159"/>
+      <c r="AM6" s="159"/>
+      <c r="AN6" s="159"/>
+      <c r="AO6" s="159"/>
+      <c r="AP6" s="159"/>
+      <c r="AQ6" s="159"/>
+      <c r="AR6" s="159"/>
+      <c r="AS6" s="159"/>
+      <c r="AT6" s="159"/>
+      <c r="AU6" s="159"/>
+      <c r="AV6" s="159"/>
+      <c r="AW6" s="159"/>
+      <c r="AX6" s="159"/>
+      <c r="AY6" s="159"/>
+      <c r="AZ6" s="159"/>
+      <c r="BA6" s="159"/>
+      <c r="BB6" s="159"/>
+      <c r="BC6" s="159"/>
+      <c r="BD6" s="159"/>
+      <c r="BE6" s="159"/>
+      <c r="BF6" s="159"/>
+      <c r="BG6" s="159"/>
+      <c r="BH6" s="159"/>
+      <c r="BI6" s="159"/>
+      <c r="BJ6" s="160"/>
+      <c r="BK6" s="162">
         <v>11</v>
       </c>
-      <c r="BL6" s="143"/>
-      <c r="BM6" s="143"/>
-      <c r="BN6" s="143"/>
-      <c r="BO6" s="143"/>
-      <c r="BP6" s="143"/>
-      <c r="BQ6" s="143"/>
-      <c r="BR6" s="143"/>
-      <c r="BS6" s="143"/>
-      <c r="BT6" s="143"/>
-      <c r="BU6" s="143"/>
-      <c r="BV6" s="143"/>
-      <c r="BW6" s="143"/>
-      <c r="BX6" s="143"/>
-      <c r="BY6" s="143"/>
-      <c r="BZ6" s="143"/>
-      <c r="CA6" s="143"/>
-      <c r="CB6" s="143"/>
-      <c r="CC6" s="143"/>
-      <c r="CD6" s="143"/>
-      <c r="CE6" s="143"/>
-      <c r="CF6" s="143"/>
-      <c r="CG6" s="143"/>
-      <c r="CH6" s="143"/>
-      <c r="CI6" s="143"/>
-      <c r="CJ6" s="143"/>
-      <c r="CK6" s="143"/>
-      <c r="CL6" s="143"/>
-      <c r="CM6" s="143"/>
-      <c r="CN6" s="144"/>
-      <c r="CO6" s="139">
+      <c r="BL6" s="163"/>
+      <c r="BM6" s="163"/>
+      <c r="BN6" s="163"/>
+      <c r="BO6" s="163"/>
+      <c r="BP6" s="163"/>
+      <c r="BQ6" s="163"/>
+      <c r="BR6" s="163"/>
+      <c r="BS6" s="163"/>
+      <c r="BT6" s="163"/>
+      <c r="BU6" s="163"/>
+      <c r="BV6" s="163"/>
+      <c r="BW6" s="163"/>
+      <c r="BX6" s="163"/>
+      <c r="BY6" s="163"/>
+      <c r="BZ6" s="163"/>
+      <c r="CA6" s="163"/>
+      <c r="CB6" s="163"/>
+      <c r="CC6" s="163"/>
+      <c r="CD6" s="163"/>
+      <c r="CE6" s="163"/>
+      <c r="CF6" s="163"/>
+      <c r="CG6" s="163"/>
+      <c r="CH6" s="163"/>
+      <c r="CI6" s="163"/>
+      <c r="CJ6" s="163"/>
+      <c r="CK6" s="163"/>
+      <c r="CL6" s="163"/>
+      <c r="CM6" s="163"/>
+      <c r="CN6" s="164"/>
+      <c r="CO6" s="159">
         <v>12</v>
       </c>
-      <c r="CP6" s="139"/>
-      <c r="CQ6" s="139"/>
-      <c r="CR6" s="139"/>
-      <c r="CS6" s="139"/>
-      <c r="CT6" s="139"/>
-      <c r="CU6" s="139"/>
-      <c r="CV6" s="139"/>
-      <c r="CW6" s="139"/>
-      <c r="CX6" s="139"/>
-      <c r="CY6" s="139"/>
-      <c r="CZ6" s="139"/>
-      <c r="DA6" s="139"/>
-      <c r="DB6" s="139"/>
-      <c r="DC6" s="139"/>
-      <c r="DD6" s="139"/>
-      <c r="DE6" s="139"/>
-      <c r="DF6" s="139"/>
-      <c r="DG6" s="139"/>
-      <c r="DH6" s="139"/>
-      <c r="DI6" s="139"/>
-      <c r="DJ6" s="139"/>
-      <c r="DK6" s="139"/>
-      <c r="DL6" s="139"/>
-      <c r="DM6" s="139"/>
-      <c r="DN6" s="139"/>
-      <c r="DO6" s="139"/>
-      <c r="DP6" s="139"/>
-      <c r="DQ6" s="139"/>
-      <c r="DR6" s="139"/>
-      <c r="DS6" s="140"/>
-      <c r="DT6" s="139">
+      <c r="CP6" s="159"/>
+      <c r="CQ6" s="159"/>
+      <c r="CR6" s="159"/>
+      <c r="CS6" s="159"/>
+      <c r="CT6" s="159"/>
+      <c r="CU6" s="159"/>
+      <c r="CV6" s="159"/>
+      <c r="CW6" s="159"/>
+      <c r="CX6" s="159"/>
+      <c r="CY6" s="159"/>
+      <c r="CZ6" s="159"/>
+      <c r="DA6" s="159"/>
+      <c r="DB6" s="159"/>
+      <c r="DC6" s="159"/>
+      <c r="DD6" s="159"/>
+      <c r="DE6" s="159"/>
+      <c r="DF6" s="159"/>
+      <c r="DG6" s="159"/>
+      <c r="DH6" s="159"/>
+      <c r="DI6" s="159"/>
+      <c r="DJ6" s="159"/>
+      <c r="DK6" s="159"/>
+      <c r="DL6" s="159"/>
+      <c r="DM6" s="159"/>
+      <c r="DN6" s="159"/>
+      <c r="DO6" s="159"/>
+      <c r="DP6" s="159"/>
+      <c r="DQ6" s="159"/>
+      <c r="DR6" s="159"/>
+      <c r="DS6" s="160"/>
+      <c r="DT6" s="159">
         <v>2019.01</v>
       </c>
-      <c r="DU6" s="139"/>
-      <c r="DV6" s="139"/>
-      <c r="DW6" s="139"/>
-      <c r="DX6" s="139"/>
-      <c r="DY6" s="139"/>
-      <c r="DZ6" s="139"/>
-      <c r="EA6" s="139"/>
-      <c r="EB6" s="139"/>
-      <c r="EC6" s="139"/>
-      <c r="ED6" s="139"/>
-      <c r="EE6" s="139"/>
-      <c r="EF6" s="139"/>
-      <c r="EG6" s="139"/>
-      <c r="EH6" s="139"/>
-      <c r="EI6" s="139"/>
-      <c r="EJ6" s="139"/>
-      <c r="EK6" s="139"/>
-      <c r="EL6" s="139"/>
-      <c r="EM6" s="139"/>
-      <c r="EN6" s="139"/>
-      <c r="EO6" s="139"/>
-      <c r="EP6" s="139"/>
-      <c r="EQ6" s="139"/>
-      <c r="ER6" s="139"/>
-      <c r="ES6" s="139"/>
-      <c r="ET6" s="139"/>
-      <c r="EU6" s="139"/>
-      <c r="EV6" s="139"/>
-      <c r="EW6" s="139"/>
-      <c r="EX6" s="140"/>
-      <c r="EY6" s="141">
+      <c r="DU6" s="159"/>
+      <c r="DV6" s="159"/>
+      <c r="DW6" s="159"/>
+      <c r="DX6" s="159"/>
+      <c r="DY6" s="159"/>
+      <c r="DZ6" s="159"/>
+      <c r="EA6" s="159"/>
+      <c r="EB6" s="159"/>
+      <c r="EC6" s="159"/>
+      <c r="ED6" s="159"/>
+      <c r="EE6" s="159"/>
+      <c r="EF6" s="159"/>
+      <c r="EG6" s="159"/>
+      <c r="EH6" s="159"/>
+      <c r="EI6" s="159"/>
+      <c r="EJ6" s="159"/>
+      <c r="EK6" s="159"/>
+      <c r="EL6" s="159"/>
+      <c r="EM6" s="159"/>
+      <c r="EN6" s="159"/>
+      <c r="EO6" s="159"/>
+      <c r="EP6" s="159"/>
+      <c r="EQ6" s="159"/>
+      <c r="ER6" s="159"/>
+      <c r="ES6" s="159"/>
+      <c r="ET6" s="159"/>
+      <c r="EU6" s="159"/>
+      <c r="EV6" s="159"/>
+      <c r="EW6" s="159"/>
+      <c r="EX6" s="160"/>
+      <c r="EY6" s="161">
         <v>2019.02</v>
       </c>
-      <c r="EZ6" s="139"/>
-      <c r="FA6" s="139"/>
-      <c r="FB6" s="139"/>
-      <c r="FC6" s="139"/>
-      <c r="FD6" s="139"/>
-      <c r="FE6" s="139"/>
-      <c r="FF6" s="139"/>
-      <c r="FG6" s="139"/>
-      <c r="FH6" s="139"/>
-      <c r="FI6" s="139"/>
-      <c r="FJ6" s="139"/>
-      <c r="FK6" s="139"/>
-      <c r="FL6" s="139"/>
-      <c r="FM6" s="139"/>
-      <c r="FN6" s="139"/>
-      <c r="FO6" s="139"/>
-      <c r="FP6" s="139"/>
-      <c r="FQ6" s="139"/>
-      <c r="FR6" s="139"/>
-      <c r="FS6" s="139"/>
-      <c r="FT6" s="139"/>
-      <c r="FU6" s="139"/>
-      <c r="FV6" s="139"/>
-      <c r="FW6" s="139"/>
-      <c r="FX6" s="139"/>
-      <c r="FY6" s="139"/>
-      <c r="FZ6" s="140"/>
-      <c r="GA6" s="132">
+      <c r="EZ6" s="159"/>
+      <c r="FA6" s="159"/>
+      <c r="FB6" s="159"/>
+      <c r="FC6" s="159"/>
+      <c r="FD6" s="159"/>
+      <c r="FE6" s="159"/>
+      <c r="FF6" s="159"/>
+      <c r="FG6" s="159"/>
+      <c r="FH6" s="159"/>
+      <c r="FI6" s="159"/>
+      <c r="FJ6" s="159"/>
+      <c r="FK6" s="159"/>
+      <c r="FL6" s="159"/>
+      <c r="FM6" s="159"/>
+      <c r="FN6" s="159"/>
+      <c r="FO6" s="159"/>
+      <c r="FP6" s="159"/>
+      <c r="FQ6" s="159"/>
+      <c r="FR6" s="159"/>
+      <c r="FS6" s="159"/>
+      <c r="FT6" s="159"/>
+      <c r="FU6" s="159"/>
+      <c r="FV6" s="159"/>
+      <c r="FW6" s="159"/>
+      <c r="FX6" s="159"/>
+      <c r="FY6" s="159"/>
+      <c r="FZ6" s="160"/>
+      <c r="GA6" s="152">
         <v>3</v>
       </c>
-      <c r="GB6" s="132"/>
-      <c r="GC6" s="132"/>
-      <c r="GD6" s="132"/>
-      <c r="GE6" s="132"/>
-      <c r="GF6" s="132"/>
-      <c r="GG6" s="132"/>
-      <c r="GH6" s="132"/>
-      <c r="GI6" s="132"/>
-      <c r="GJ6" s="132"/>
-      <c r="GK6" s="132"/>
-      <c r="GL6" s="132"/>
-      <c r="GM6" s="132"/>
-      <c r="GN6" s="132"/>
-      <c r="GO6" s="132"/>
-      <c r="GP6" s="132"/>
-      <c r="GQ6" s="132"/>
-      <c r="GR6" s="132"/>
-      <c r="GS6" s="132"/>
-      <c r="GT6" s="132"/>
-      <c r="GU6" s="132"/>
-      <c r="GV6" s="132"/>
-      <c r="GW6" s="132"/>
-      <c r="GX6" s="132"/>
-      <c r="GY6" s="132"/>
-      <c r="GZ6" s="132"/>
-      <c r="HA6" s="132"/>
-      <c r="HB6" s="132"/>
-      <c r="HC6" s="132"/>
-      <c r="HD6" s="132"/>
-      <c r="HE6" s="132"/>
-      <c r="HF6" s="136">
+      <c r="GB6" s="152"/>
+      <c r="GC6" s="152"/>
+      <c r="GD6" s="152"/>
+      <c r="GE6" s="152"/>
+      <c r="GF6" s="152"/>
+      <c r="GG6" s="152"/>
+      <c r="GH6" s="152"/>
+      <c r="GI6" s="152"/>
+      <c r="GJ6" s="152"/>
+      <c r="GK6" s="152"/>
+      <c r="GL6" s="152"/>
+      <c r="GM6" s="152"/>
+      <c r="GN6" s="152"/>
+      <c r="GO6" s="152"/>
+      <c r="GP6" s="152"/>
+      <c r="GQ6" s="152"/>
+      <c r="GR6" s="152"/>
+      <c r="GS6" s="152"/>
+      <c r="GT6" s="152"/>
+      <c r="GU6" s="152"/>
+      <c r="GV6" s="152"/>
+      <c r="GW6" s="152"/>
+      <c r="GX6" s="152"/>
+      <c r="GY6" s="152"/>
+      <c r="GZ6" s="152"/>
+      <c r="HA6" s="152"/>
+      <c r="HB6" s="152"/>
+      <c r="HC6" s="152"/>
+      <c r="HD6" s="152"/>
+      <c r="HE6" s="152"/>
+      <c r="HF6" s="156">
         <v>4</v>
       </c>
-      <c r="HG6" s="137"/>
-      <c r="HH6" s="137"/>
-      <c r="HI6" s="137"/>
-      <c r="HJ6" s="137"/>
-      <c r="HK6" s="137"/>
-      <c r="HL6" s="137"/>
-      <c r="HM6" s="137"/>
-      <c r="HN6" s="137"/>
-      <c r="HO6" s="137"/>
-      <c r="HP6" s="137"/>
-      <c r="HQ6" s="137"/>
-      <c r="HR6" s="137"/>
-      <c r="HS6" s="137"/>
-      <c r="HT6" s="137"/>
-      <c r="HU6" s="137"/>
-      <c r="HV6" s="137"/>
-      <c r="HW6" s="137"/>
-      <c r="HX6" s="137"/>
-      <c r="HY6" s="137"/>
-      <c r="HZ6" s="137"/>
-      <c r="IA6" s="137"/>
-      <c r="IB6" s="137"/>
-      <c r="IC6" s="137"/>
-      <c r="ID6" s="137"/>
-      <c r="IE6" s="137"/>
-      <c r="IF6" s="137"/>
-      <c r="IG6" s="137"/>
-      <c r="IH6" s="137"/>
-      <c r="II6" s="138"/>
-      <c r="IJ6" s="131">
+      <c r="HG6" s="157"/>
+      <c r="HH6" s="157"/>
+      <c r="HI6" s="157"/>
+      <c r="HJ6" s="157"/>
+      <c r="HK6" s="157"/>
+      <c r="HL6" s="157"/>
+      <c r="HM6" s="157"/>
+      <c r="HN6" s="157"/>
+      <c r="HO6" s="157"/>
+      <c r="HP6" s="157"/>
+      <c r="HQ6" s="157"/>
+      <c r="HR6" s="157"/>
+      <c r="HS6" s="157"/>
+      <c r="HT6" s="157"/>
+      <c r="HU6" s="157"/>
+      <c r="HV6" s="157"/>
+      <c r="HW6" s="157"/>
+      <c r="HX6" s="157"/>
+      <c r="HY6" s="157"/>
+      <c r="HZ6" s="157"/>
+      <c r="IA6" s="157"/>
+      <c r="IB6" s="157"/>
+      <c r="IC6" s="157"/>
+      <c r="ID6" s="157"/>
+      <c r="IE6" s="157"/>
+      <c r="IF6" s="157"/>
+      <c r="IG6" s="157"/>
+      <c r="IH6" s="157"/>
+      <c r="II6" s="158"/>
+      <c r="IJ6" s="151">
         <v>5</v>
       </c>
-      <c r="IK6" s="132"/>
-      <c r="IL6" s="132"/>
-      <c r="IM6" s="132"/>
-      <c r="IN6" s="132"/>
-      <c r="IO6" s="132"/>
-      <c r="IP6" s="132"/>
-      <c r="IQ6" s="132"/>
-      <c r="IR6" s="132"/>
-      <c r="IS6" s="132"/>
-      <c r="IT6" s="132"/>
-      <c r="IU6" s="132"/>
-      <c r="IV6" s="132"/>
-      <c r="IW6" s="132"/>
-      <c r="IX6" s="132"/>
-      <c r="IY6" s="132"/>
-      <c r="IZ6" s="132"/>
-      <c r="JA6" s="132"/>
-      <c r="JB6" s="132"/>
-      <c r="JC6" s="132"/>
-      <c r="JD6" s="132"/>
-      <c r="JE6" s="132"/>
-      <c r="JF6" s="132"/>
-      <c r="JG6" s="132"/>
-      <c r="JH6" s="132"/>
-      <c r="JI6" s="132"/>
-      <c r="JJ6" s="132"/>
-      <c r="JK6" s="132"/>
-      <c r="JL6" s="132"/>
-      <c r="JM6" s="132"/>
-      <c r="JN6" s="133"/>
+      <c r="IK6" s="152"/>
+      <c r="IL6" s="152"/>
+      <c r="IM6" s="152"/>
+      <c r="IN6" s="152"/>
+      <c r="IO6" s="152"/>
+      <c r="IP6" s="152"/>
+      <c r="IQ6" s="152"/>
+      <c r="IR6" s="152"/>
+      <c r="IS6" s="152"/>
+      <c r="IT6" s="152"/>
+      <c r="IU6" s="152"/>
+      <c r="IV6" s="152"/>
+      <c r="IW6" s="152"/>
+      <c r="IX6" s="152"/>
+      <c r="IY6" s="152"/>
+      <c r="IZ6" s="152"/>
+      <c r="JA6" s="152"/>
+      <c r="JB6" s="152"/>
+      <c r="JC6" s="152"/>
+      <c r="JD6" s="152"/>
+      <c r="JE6" s="152"/>
+      <c r="JF6" s="152"/>
+      <c r="JG6" s="152"/>
+      <c r="JH6" s="152"/>
+      <c r="JI6" s="152"/>
+      <c r="JJ6" s="152"/>
+      <c r="JK6" s="152"/>
+      <c r="JL6" s="152"/>
+      <c r="JM6" s="152"/>
+      <c r="JN6" s="153"/>
     </row>
-    <row r="7" spans="1:274" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:274" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="53"/>
       <c r="B7" s="56">
         <v>1</v>
@@ -3727,9 +3711,9 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="134" t="s">
-        <v>29</v>
+    <row r="8" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="154" t="s">
+        <v>28</v>
       </c>
       <c r="B8" s="42"/>
       <c r="C8" s="42"/>
@@ -3861,7 +3845,9 @@
       <c r="DU8" s="9"/>
       <c r="DV8" s="9"/>
       <c r="DW8" s="9"/>
-      <c r="DX8" s="42"/>
+      <c r="DX8" s="150" t="s">
+        <v>49</v>
+      </c>
       <c r="DY8" s="42"/>
       <c r="DZ8" s="9"/>
       <c r="EA8" s="9"/>
@@ -3878,7 +3864,7 @@
       <c r="EL8" s="42"/>
       <c r="EM8" s="42"/>
       <c r="EN8" s="118" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="EO8" s="9"/>
       <c r="EP8" s="9"/>
@@ -3927,7 +3913,7 @@
       <c r="GG8" s="8"/>
       <c r="GH8" s="8"/>
       <c r="GI8" s="128" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="GJ8" s="10"/>
       <c r="GK8" s="8"/>
@@ -4013,8 +3999,8 @@
       <c r="JM8" s="8"/>
       <c r="JN8" s="40"/>
     </row>
-    <row r="9" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="134"/>
+    <row r="9" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="154"/>
       <c r="B9" s="73"/>
       <c r="C9" s="74"/>
       <c r="D9" s="75"/>
@@ -4183,7 +4169,7 @@
       <c r="FG9" s="74"/>
       <c r="FH9" s="74"/>
       <c r="FI9" s="75" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="FJ9" s="75"/>
       <c r="FK9" s="75"/>
@@ -4199,7 +4185,7 @@
       <c r="FU9" s="74"/>
       <c r="FV9" s="74"/>
       <c r="FW9" s="75" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="FX9" s="75"/>
       <c r="FY9" s="75"/>
@@ -4208,7 +4194,7 @@
       <c r="GB9" s="6"/>
       <c r="GC9" s="6"/>
       <c r="GD9" s="75" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="GE9" s="5"/>
       <c r="GF9" s="5"/>
@@ -4299,8 +4285,8 @@
       <c r="JM9" s="5"/>
       <c r="JN9" s="7"/>
     </row>
-    <row r="10" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="134"/>
+    <row r="10" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="154"/>
       <c r="B10" s="73"/>
       <c r="C10" s="74"/>
       <c r="D10" s="75"/>
@@ -4415,7 +4401,7 @@
       <c r="DI10" s="75"/>
       <c r="DJ10" s="74"/>
       <c r="DK10" s="117" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="DL10" s="75"/>
       <c r="DM10" s="117"/>
@@ -4577,8 +4563,8 @@
       <c r="JM10" s="5"/>
       <c r="JN10" s="7"/>
     </row>
-    <row r="11" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="134"/>
+    <row r="11" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="154"/>
       <c r="B11" s="73"/>
       <c r="C11" s="74"/>
       <c r="D11" s="75"/>
@@ -4698,7 +4684,9 @@
       <c r="DN11" s="75"/>
       <c r="DO11" s="75"/>
       <c r="DP11" s="75"/>
-      <c r="DQ11" s="74"/>
+      <c r="DQ11" s="74" t="s">
+        <v>47</v>
+      </c>
       <c r="DR11" s="74"/>
       <c r="DS11" s="79"/>
       <c r="DT11" s="80"/>
@@ -4853,8 +4841,8 @@
       <c r="JM11" s="5"/>
       <c r="JN11" s="7"/>
     </row>
-    <row r="12" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="134"/>
+    <row r="12" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="154"/>
       <c r="B12" s="73"/>
       <c r="C12" s="74"/>
       <c r="D12" s="75"/>
@@ -4974,7 +4962,9 @@
       <c r="DN12" s="75"/>
       <c r="DO12" s="75"/>
       <c r="DP12" s="75"/>
-      <c r="DQ12" s="74"/>
+      <c r="DQ12" s="74" t="s">
+        <v>48</v>
+      </c>
       <c r="DR12" s="74"/>
       <c r="DS12" s="79"/>
       <c r="DT12" s="80"/>
@@ -5129,8 +5119,8 @@
       <c r="JM12" s="5"/>
       <c r="JN12" s="7"/>
     </row>
-    <row r="13" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="134"/>
+    <row r="13" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="154"/>
       <c r="B13" s="73"/>
       <c r="C13" s="74"/>
       <c r="D13" s="75"/>
@@ -5405,8 +5395,8 @@
       <c r="JM13" s="5"/>
       <c r="JN13" s="7"/>
     </row>
-    <row r="14" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="134"/>
+    <row r="14" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="154"/>
       <c r="B14" s="81"/>
       <c r="C14" s="82"/>
       <c r="D14" s="83"/>
@@ -5681,8 +5671,8 @@
       <c r="JM14" s="14"/>
       <c r="JN14" s="18"/>
     </row>
-    <row r="15" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="135" t="s">
+    <row r="15" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="155" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="89"/>
@@ -5961,8 +5951,8 @@
       <c r="JM15" s="26"/>
       <c r="JN15" s="29"/>
     </row>
-    <row r="16" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="134"/>
+    <row r="16" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="154"/>
       <c r="B16" s="95"/>
       <c r="C16" s="96"/>
       <c r="D16" s="97"/>
@@ -6083,9 +6073,6 @@
       <c r="DM16" s="98"/>
       <c r="DN16" s="97"/>
       <c r="DO16" s="97"/>
-      <c r="DP16" s="100" t="s">
-        <v>6</v>
-      </c>
       <c r="DQ16" s="96"/>
       <c r="DR16" s="96"/>
       <c r="DS16" s="46"/>
@@ -6095,13 +6082,12 @@
       <c r="DW16" s="97"/>
       <c r="DX16" s="96"/>
       <c r="DY16" s="96"/>
-      <c r="DZ16" s="97" t="s">
-        <v>11</v>
-      </c>
       <c r="EA16" s="97"/>
       <c r="EB16" s="97"/>
       <c r="EC16" s="97"/>
-      <c r="ED16" s="97"/>
+      <c r="ED16" s="100" t="s">
+        <v>6</v>
+      </c>
       <c r="EE16" s="96"/>
       <c r="EF16" s="96"/>
       <c r="EG16" s="97"/>
@@ -6111,7 +6097,9 @@
       <c r="EK16" s="97"/>
       <c r="EL16" s="96"/>
       <c r="EM16" s="96"/>
-      <c r="EN16" s="97"/>
+      <c r="EN16" s="97" t="s">
+        <v>11</v>
+      </c>
       <c r="EO16" s="97"/>
       <c r="EP16" s="97"/>
       <c r="EQ16" s="97"/>
@@ -6243,8 +6231,8 @@
       <c r="JM16" s="11"/>
       <c r="JN16" s="13"/>
     </row>
-    <row r="17" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="134"/>
+    <row r="17" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="154"/>
       <c r="B17" s="95"/>
       <c r="C17" s="96"/>
       <c r="D17" s="97"/>
@@ -6363,9 +6351,6 @@
       <c r="DM17" s="98"/>
       <c r="DN17" s="97"/>
       <c r="DO17" s="97"/>
-      <c r="DP17" s="100" t="s">
-        <v>10</v>
-      </c>
       <c r="DQ17" s="96"/>
       <c r="DR17" s="96"/>
       <c r="DS17" s="97"/>
@@ -6379,7 +6364,9 @@
       <c r="EA17" s="97"/>
       <c r="EB17" s="97"/>
       <c r="EC17" s="97"/>
-      <c r="ED17" s="97"/>
+      <c r="ED17" s="100" t="s">
+        <v>10</v>
+      </c>
       <c r="EE17" s="96"/>
       <c r="EF17" s="96"/>
       <c r="EG17" s="97"/>
@@ -6521,8 +6508,8 @@
       <c r="JM17" s="2"/>
       <c r="JN17" s="4"/>
     </row>
-    <row r="18" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="134"/>
+    <row r="18" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="154"/>
       <c r="B18" s="95"/>
       <c r="C18" s="96"/>
       <c r="D18" s="97"/>
@@ -6658,9 +6645,6 @@
       <c r="ED18" s="97"/>
       <c r="EE18" s="96"/>
       <c r="EF18" s="96"/>
-      <c r="EG18" s="97" t="s">
-        <v>7</v>
-      </c>
       <c r="EH18" s="97"/>
       <c r="EI18" s="97"/>
       <c r="EJ18" s="97"/>
@@ -6674,7 +6658,9 @@
       <c r="ER18" s="97"/>
       <c r="ES18" s="96"/>
       <c r="ET18" s="96"/>
-      <c r="EU18" s="97"/>
+      <c r="EU18" s="97" t="s">
+        <v>7</v>
+      </c>
       <c r="EV18" s="97"/>
       <c r="EW18" s="97"/>
       <c r="EX18" s="46"/>
@@ -6799,8 +6785,8 @@
       <c r="JM18" s="2"/>
       <c r="JN18" s="4"/>
     </row>
-    <row r="19" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="134"/>
+    <row r="19" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="154"/>
       <c r="B19" s="95"/>
       <c r="C19" s="96"/>
       <c r="D19" s="97"/>
@@ -7075,8 +7061,8 @@
       <c r="JM19" s="2"/>
       <c r="JN19" s="4"/>
     </row>
-    <row r="20" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="134"/>
+    <row r="20" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="154"/>
       <c r="B20" s="95"/>
       <c r="C20" s="96"/>
       <c r="D20" s="97"/>
@@ -7351,8 +7337,8 @@
       <c r="JM20" s="2"/>
       <c r="JN20" s="4"/>
     </row>
-    <row r="21" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="134"/>
+    <row r="21" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="154"/>
       <c r="B21" s="95"/>
       <c r="C21" s="96"/>
       <c r="D21" s="97"/>
@@ -7627,8 +7613,8 @@
       <c r="JM21" s="125"/>
       <c r="JN21" s="127"/>
     </row>
-    <row r="22" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="134"/>
+    <row r="22" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="154"/>
       <c r="B22" s="102"/>
       <c r="C22" s="103"/>
       <c r="D22" s="104"/>
@@ -7903,9 +7889,9 @@
       <c r="JM22" s="23"/>
       <c r="JN22" s="25"/>
     </row>
-    <row r="23" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="134" t="s">
-        <v>30</v>
+    <row r="23" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="154" t="s">
+        <v>29</v>
       </c>
       <c r="B23" s="108"/>
       <c r="C23" s="109"/>
@@ -8060,7 +8046,7 @@
       <c r="EV23" s="110"/>
       <c r="EW23" s="110"/>
       <c r="EX23" s="118" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="EY23" s="113"/>
       <c r="EZ23" s="109"/>
@@ -8183,8 +8169,8 @@
       <c r="JM23" s="26"/>
       <c r="JN23" s="29"/>
     </row>
-    <row r="24" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="134"/>
+    <row r="24" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="154"/>
       <c r="B24" s="95"/>
       <c r="C24" s="96"/>
       <c r="D24" s="97"/>
@@ -8339,7 +8325,7 @@
       <c r="EW24" s="97"/>
       <c r="EX24" s="46"/>
       <c r="EY24" s="99" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="EZ24" s="96"/>
       <c r="FA24" s="96"/>
@@ -8461,8 +8447,8 @@
       <c r="JM24" s="2"/>
       <c r="JN24" s="4"/>
     </row>
-    <row r="25" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="134"/>
+    <row r="25" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="154"/>
       <c r="B25" s="95"/>
       <c r="C25" s="96"/>
       <c r="D25" s="97"/>
@@ -8623,7 +8609,7 @@
       <c r="FC25" s="98"/>
       <c r="FD25" s="98"/>
       <c r="FE25" s="100" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="FF25" s="100"/>
       <c r="FG25" s="96"/>
@@ -8739,8 +8725,8 @@
       <c r="JM25" s="2"/>
       <c r="JN25" s="4"/>
     </row>
-    <row r="26" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="134"/>
+    <row r="26" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="154"/>
       <c r="B26" s="95"/>
       <c r="C26" s="96"/>
       <c r="D26" s="97"/>
@@ -8905,7 +8891,7 @@
       <c r="FG26" s="96"/>
       <c r="FH26" s="96"/>
       <c r="FI26" s="75" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="FJ26" s="97"/>
       <c r="FK26" s="97"/>
@@ -8921,7 +8907,7 @@
       <c r="FU26" s="96"/>
       <c r="FV26" s="96"/>
       <c r="FW26" s="75" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="FX26" s="97"/>
       <c r="FY26" s="97"/>
@@ -8937,13 +8923,13 @@
       <c r="GI26" s="1"/>
       <c r="GJ26" s="1"/>
       <c r="GK26" s="75" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="GL26" s="2"/>
       <c r="GM26" s="2"/>
       <c r="GN26" s="2"/>
       <c r="GO26" s="75" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="GP26" s="1"/>
       <c r="GQ26" s="1"/>
@@ -9023,8 +9009,8 @@
       <c r="JM26" s="2"/>
       <c r="JN26" s="4"/>
     </row>
-    <row r="27" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="134"/>
+    <row r="27" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="154"/>
       <c r="B27" s="95"/>
       <c r="C27" s="96"/>
       <c r="D27" s="97"/>
@@ -9194,7 +9180,7 @@
       <c r="FL27" s="97"/>
       <c r="FM27" s="97"/>
       <c r="FN27" s="96" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="FO27" s="96"/>
       <c r="FP27" s="97"/>
@@ -9205,7 +9191,7 @@
       <c r="FU27" s="96"/>
       <c r="FV27" s="96"/>
       <c r="FW27" s="75" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="FX27" s="97"/>
       <c r="FY27" s="97"/>
@@ -9305,8 +9291,8 @@
       <c r="JM27" s="2"/>
       <c r="JN27" s="4"/>
     </row>
-    <row r="28" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="134"/>
+    <row r="28" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="154"/>
       <c r="B28" s="95"/>
       <c r="C28" s="96"/>
       <c r="D28" s="97"/>
@@ -9485,7 +9471,7 @@
       <c r="FU28" s="96"/>
       <c r="FV28" s="96"/>
       <c r="FW28" s="75" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="FX28" s="97"/>
       <c r="FY28" s="97"/>
@@ -9583,8 +9569,8 @@
       <c r="JM28" s="2"/>
       <c r="JN28" s="4"/>
     </row>
-    <row r="29" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="134"/>
+    <row r="29" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="154"/>
       <c r="B29" s="95"/>
       <c r="C29" s="96"/>
       <c r="D29" s="97"/>
@@ -9763,7 +9749,7 @@
       <c r="FU29" s="96"/>
       <c r="FV29" s="96"/>
       <c r="FW29" s="75" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="FX29" s="97"/>
       <c r="FY29" s="97"/>
@@ -9861,8 +9847,8 @@
       <c r="JM29" s="2"/>
       <c r="JN29" s="4"/>
     </row>
-    <row r="30" spans="1:274" ht="16.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="134"/>
+    <row r="30" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="154"/>
       <c r="B30" s="102"/>
       <c r="C30" s="103"/>
       <c r="D30" s="104"/>
@@ -10137,19 +10123,19 @@
       <c r="JM30" s="23"/>
       <c r="JN30" s="25"/>
     </row>
-    <row r="31" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="48"/>
     </row>
-    <row r="32" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="48"/>
     </row>
-    <row r="33" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="48"/>
     </row>
-    <row r="34" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="48"/>
     </row>
-    <row r="35" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="48"/>
       <c r="GA35" s="55"/>
       <c r="GB35" s="55"/>
@@ -10244,7 +10230,7 @@
       <c r="JM35" s="55"/>
       <c r="JN35" s="55"/>
     </row>
-    <row r="36" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="48"/>
       <c r="GA36" s="55"/>
       <c r="GB36" s="55"/>
@@ -10339,7 +10325,7 @@
       <c r="JM36" s="55"/>
       <c r="JN36" s="55"/>
     </row>
-    <row r="37" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="48"/>
       <c r="GA37" s="55"/>
       <c r="GB37" s="55"/>
@@ -10434,7 +10420,7 @@
       <c r="JM37" s="55"/>
       <c r="JN37" s="55"/>
     </row>
-    <row r="38" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="48"/>
       <c r="GA38" s="55"/>
       <c r="GB38" s="55"/>
@@ -10529,7 +10515,7 @@
       <c r="JM38" s="55"/>
       <c r="JN38" s="55"/>
     </row>
-    <row r="39" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="48"/>
       <c r="GA39" s="55"/>
       <c r="GB39" s="55"/>
@@ -10624,7 +10610,7 @@
       <c r="JM39" s="55"/>
       <c r="JN39" s="55"/>
     </row>
-    <row r="40" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="48"/>
       <c r="GA40" s="55"/>
       <c r="GB40" s="55"/>
@@ -10719,7 +10705,7 @@
       <c r="JM40" s="55"/>
       <c r="JN40" s="55"/>
     </row>
-    <row r="41" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="48"/>
       <c r="GA41" s="55"/>
       <c r="GB41" s="55"/>
@@ -10814,7 +10800,7 @@
       <c r="JM41" s="55"/>
       <c r="JN41" s="55"/>
     </row>
-    <row r="42" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="48"/>
       <c r="GA42" s="55"/>
       <c r="GB42" s="55"/>
@@ -10909,7 +10895,7 @@
       <c r="JM42" s="55"/>
       <c r="JN42" s="55"/>
     </row>
-    <row r="43" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="48"/>
       <c r="GA43" s="55"/>
       <c r="GB43" s="55"/>
@@ -11004,7 +10990,7 @@
       <c r="JM43" s="55"/>
       <c r="JN43" s="55"/>
     </row>
-    <row r="44" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="48"/>
       <c r="GA44" s="55"/>
       <c r="GB44" s="55"/>
@@ -11099,7 +11085,7 @@
       <c r="JM44" s="55"/>
       <c r="JN44" s="55"/>
     </row>
-    <row r="45" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="48"/>
       <c r="GA45" s="55"/>
       <c r="GB45" s="55"/>
@@ -11194,7 +11180,7 @@
       <c r="JM45" s="55"/>
       <c r="JN45" s="55"/>
     </row>
-    <row r="46" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="48"/>
       <c r="GA46" s="55"/>
       <c r="GB46" s="55"/>
@@ -11289,7 +11275,7 @@
       <c r="JM46" s="55"/>
       <c r="JN46" s="55"/>
     </row>
-    <row r="47" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:274" s="54" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="48"/>
       <c r="GA47" s="55"/>
       <c r="GB47" s="55"/>
@@ -11408,245 +11394,253 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8DA35E3-DBFD-486D-BF52-F3E372F58B68}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.796875" style="146"/>
-    <col min="3" max="3" width="4.69921875" style="146" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.69921875" style="146" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.796875" customWidth="1"/>
+    <col min="2" max="2" width="8.75" style="132"/>
+    <col min="3" max="3" width="4.75" style="132" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.75" style="132" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="146" t="s">
+    <row r="2" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="132" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="146" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="147" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="148" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="149" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="165" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="166" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="167" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="168" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="155">
+    <row r="4" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="165">
         <v>2018.12</v>
       </c>
-      <c r="C4" s="156"/>
-      <c r="D4" s="153">
+      <c r="C4" s="166"/>
+      <c r="D4" s="139">
         <f>SUM(D5:D13)</f>
         <v>42</v>
       </c>
-      <c r="E4" s="154"/>
+      <c r="E4" s="140"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B5" s="157">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="167">
         <v>12</v>
       </c>
-      <c r="C5" s="160">
+      <c r="C5" s="143">
         <v>7</v>
       </c>
-      <c r="D5" s="160">
+      <c r="D5" s="143">
         <v>4</v>
       </c>
-      <c r="E5" s="161" t="s">
-        <v>46</v>
+      <c r="E5" s="144" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B6" s="162"/>
-      <c r="C6" s="158">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="168"/>
+      <c r="C6" s="141">
         <v>17</v>
       </c>
-      <c r="D6" s="158">
+      <c r="D6" s="141">
         <v>4</v>
       </c>
-      <c r="E6" s="163" t="s">
-        <v>45</v>
+      <c r="E6" s="145" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B7" s="162"/>
-      <c r="C7" s="158">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="168"/>
+      <c r="C7" s="141">
         <v>19</v>
       </c>
-      <c r="D7" s="158">
+      <c r="D7" s="141">
         <v>8</v>
       </c>
-      <c r="E7" s="163" t="s">
-        <v>45</v>
+      <c r="E7" s="145" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B8" s="162"/>
-      <c r="C8" s="148">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="168"/>
+      <c r="C8" s="134">
         <v>22</v>
       </c>
-      <c r="D8" s="148">
+      <c r="D8" s="134">
         <v>3</v>
       </c>
       <c r="E8" s="129" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="168"/>
+      <c r="C9" s="134">
+        <v>23</v>
+      </c>
+      <c r="D9" s="134">
+        <v>6</v>
+      </c>
+      <c r="E9" s="129" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="168"/>
+      <c r="C10" s="134">
+        <v>25</v>
+      </c>
+      <c r="D10" s="134">
+        <v>8</v>
+      </c>
+      <c r="E10" s="129" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B9" s="162"/>
-      <c r="C9" s="148">
-        <v>23</v>
-      </c>
-      <c r="D9" s="148">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="168"/>
+      <c r="C11" s="134">
+        <v>26</v>
+      </c>
+      <c r="D11" s="134">
+        <v>5</v>
+      </c>
+      <c r="E11" s="129" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="33" x14ac:dyDescent="0.3">
+      <c r="B12" s="168"/>
+      <c r="C12" s="134">
+        <v>29</v>
+      </c>
+      <c r="D12" s="134">
+        <v>2</v>
+      </c>
+      <c r="E12" s="131" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="169"/>
+      <c r="C13" s="137">
+        <v>30</v>
+      </c>
+      <c r="D13" s="137">
+        <v>2</v>
+      </c>
+      <c r="E13" s="130" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="165">
+        <v>2019.01</v>
+      </c>
+      <c r="C14" s="166"/>
+      <c r="D14" s="139">
+        <f>SUM(D15:D22)</f>
+        <v>11</v>
+      </c>
+      <c r="E14" s="142"/>
+    </row>
+    <row r="15" spans="2:5" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B15" s="133">
+        <v>1</v>
+      </c>
+      <c r="C15" s="134">
+        <v>1</v>
+      </c>
+      <c r="D15" s="135">
         <v>6</v>
       </c>
-      <c r="E9" s="129" t="s">
-        <v>28</v>
+      <c r="E15" s="131" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B10" s="162"/>
-      <c r="C10" s="148">
-        <v>25</v>
-      </c>
-      <c r="D10" s="148">
-        <v>8</v>
-      </c>
-      <c r="E10" s="129" t="s">
-        <v>27</v>
+    <row r="16" spans="2:5" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B16" s="133">
+        <v>1</v>
+      </c>
+      <c r="C16" s="134">
+        <v>5</v>
+      </c>
+      <c r="D16" s="135">
+        <v>5</v>
+      </c>
+      <c r="E16" s="131" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B11" s="162"/>
-      <c r="C11" s="148">
-        <v>26</v>
-      </c>
-      <c r="D11" s="148">
-        <v>5</v>
-      </c>
-      <c r="E11" s="129" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="B12" s="162"/>
-      <c r="C12" s="148">
-        <v>29</v>
-      </c>
-      <c r="D12" s="148">
-        <v>2</v>
-      </c>
-      <c r="E12" s="145" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="164"/>
-      <c r="C13" s="151">
-        <v>30</v>
-      </c>
-      <c r="D13" s="151">
-        <v>2</v>
-      </c>
-      <c r="E13" s="130" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B14" s="155">
-        <v>2019.01</v>
-      </c>
-      <c r="C14" s="156"/>
-      <c r="D14" s="153">
-        <f>SUM(D15:D22)</f>
-        <v>6</v>
-      </c>
-      <c r="E14" s="159"/>
-    </row>
-    <row r="15" spans="2:5" ht="52.2" x14ac:dyDescent="0.4">
-      <c r="B15" s="147">
-        <v>1</v>
-      </c>
-      <c r="C15" s="148">
-        <v>1</v>
-      </c>
-      <c r="D15" s="149">
-        <v>6</v>
-      </c>
-      <c r="E15" s="145" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B16" s="147"/>
-      <c r="C16" s="148"/>
-      <c r="D16" s="149"/>
-      <c r="E16" s="129"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B17" s="147"/>
-      <c r="C17" s="148"/>
-      <c r="D17" s="149"/>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="133"/>
+      <c r="C17" s="134"/>
+      <c r="D17" s="135"/>
       <c r="E17" s="129"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B18" s="147"/>
-      <c r="C18" s="148"/>
-      <c r="D18" s="149"/>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="133"/>
+      <c r="C18" s="134"/>
+      <c r="D18" s="135"/>
       <c r="E18" s="129"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B19" s="147"/>
-      <c r="C19" s="148"/>
-      <c r="D19" s="149"/>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="133"/>
+      <c r="C19" s="134"/>
+      <c r="D19" s="135"/>
       <c r="E19" s="129"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B20" s="147"/>
-      <c r="C20" s="148"/>
-      <c r="D20" s="149"/>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="133"/>
+      <c r="C20" s="134"/>
+      <c r="D20" s="135"/>
       <c r="E20" s="129"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B21" s="147"/>
-      <c r="C21" s="148"/>
-      <c r="D21" s="149"/>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="133"/>
+      <c r="C21" s="134"/>
+      <c r="D21" s="135"/>
       <c r="E21" s="129"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B22" s="147"/>
-      <c r="C22" s="148"/>
-      <c r="D22" s="149"/>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="133"/>
+      <c r="C22" s="134"/>
+      <c r="D22" s="135"/>
       <c r="E22" s="129"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B23" s="147"/>
-      <c r="C23" s="148"/>
-      <c r="D23" s="149"/>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="133"/>
+      <c r="C23" s="134"/>
+      <c r="D23" s="135"/>
       <c r="E23" s="129"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B24" s="147"/>
-      <c r="C24" s="148"/>
-      <c r="D24" s="149"/>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="133"/>
+      <c r="C24" s="134"/>
+      <c r="D24" s="135"/>
       <c r="E24" s="129"/>
     </row>
-    <row r="25" spans="2:5" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B25" s="150"/>
-      <c r="C25" s="151"/>
-      <c r="D25" s="152"/>
+    <row r="25" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="136"/>
+      <c r="C25" s="137"/>
+      <c r="D25" s="138"/>
       <c r="E25" s="130"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[DOC] Pipette, RF Gen work update
</commit_message>
<xml_diff>
--- a/Plasma Project schedule V1.0.xlsx
+++ b/Plasma Project schedule V1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="20181224" sheetId="20" r:id="rId1"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>Femto Project 일정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -361,12 +361,28 @@
     <t>MPD review</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>◇ Femto Meeting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Femto meeting - Battery 동작 설명/ MPD cable 제작 설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF Generator SCH review</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF Generator Sch &amp; PCB 완료</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,6 +486,21 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -503,7 +534,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="51">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -1127,11 +1158,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1351,6 +1404,13 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1399,6 +1459,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1408,6 +1474,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1416,8 +1484,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
       <color rgb="FFFF66FF"/>
-      <color rgb="FF0000FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1451,7 +1519,7 @@
         <xdr:cNvPr id="52" name="직선 화살표 연결선 51">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000034000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1508,7 +1576,7 @@
         <xdr:cNvPr id="15" name="직선 화살표 연결선 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1565,7 +1633,7 @@
         <xdr:cNvPr id="18" name="직선 화살표 연결선 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B9B7B3B-4B32-4051-898C-EE6F25736D05}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B9B7B3B-4B32-4051-898C-EE6F25736D05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1581,7 +1649,7 @@
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:srgbClr val="0000FF"/>
+            <a:srgbClr val="FF0000"/>
           </a:solidFill>
           <a:prstDash val="sysDash"/>
           <a:tailEnd type="triangle"/>
@@ -1622,7 +1690,7 @@
         <xdr:cNvPr id="21" name="직선 화살표 연결선 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEEB29C9-2143-40DD-9242-A82E285F4B2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CEEB29C9-2143-40DD-9242-A82E285F4B2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1638,7 +1706,7 @@
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:srgbClr val="0000FF"/>
+            <a:srgbClr val="FF0000"/>
           </a:solidFill>
           <a:prstDash val="sysDash"/>
           <a:tailEnd type="triangle"/>
@@ -1679,7 +1747,7 @@
         <xdr:cNvPr id="25" name="직선 화살표 연결선 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2375196F-31DF-4BFC-AC62-19AF714F443A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2375196F-31DF-4BFC-AC62-19AF714F443A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1736,7 +1804,7 @@
         <xdr:cNvPr id="28" name="직선 화살표 연결선 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D1266C4-6D7E-4F8B-8103-59BF7C6FE4FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3D1266C4-6D7E-4F8B-8103-59BF7C6FE4FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1793,7 +1861,7 @@
         <xdr:cNvPr id="32" name="직선 화살표 연결선 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{666CF52C-5D68-4474-8BDD-79976E036787}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{666CF52C-5D68-4474-8BDD-79976E036787}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1850,7 +1918,7 @@
         <xdr:cNvPr id="33" name="직선 화살표 연결선 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07D67EB1-AD43-42F4-B443-3BB978B9F2AC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{07D67EB1-AD43-42F4-B443-3BB978B9F2AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1907,7 +1975,7 @@
         <xdr:cNvPr id="36" name="직선 화살표 연결선 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A732A08-4D4F-441D-9243-033ACD4A7F32}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9A732A08-4D4F-441D-9243-033ACD4A7F32}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1923,7 +1991,7 @@
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
-            <a:srgbClr val="0000FF"/>
+            <a:srgbClr val="FF0000"/>
           </a:solidFill>
           <a:prstDash val="sysDash"/>
           <a:tailEnd type="triangle"/>
@@ -1964,7 +2032,7 @@
         <xdr:cNvPr id="38" name="직선 화살표 연결선 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A864090-2577-47BA-8983-FFA17538A224}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3A864090-2577-47BA-8983-FFA17538A224}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2021,7 +2089,7 @@
         <xdr:cNvPr id="41" name="직선 화살표 연결선 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B9CC53C-2611-4F5F-B122-A3165CFAFB90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B9CC53C-2611-4F5F-B122-A3165CFAFB90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2078,7 +2146,7 @@
         <xdr:cNvPr id="46" name="직선 화살표 연결선 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6CC6FD7-49CF-4859-9978-820DB474FDCC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A6CC6FD7-49CF-4859-9978-820DB474FDCC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2135,7 +2203,7 @@
         <xdr:cNvPr id="14" name="직선 화살표 연결선 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5A7DBF8-E685-466C-85D3-36D1828C9CBD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A5A7DBF8-E685-466C-85D3-36D1828C9CBD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2192,7 +2260,7 @@
         <xdr:cNvPr id="16" name="직선 화살표 연결선 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D724AD7-DEC3-4BAD-A0BE-EBB685097DA0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8D724AD7-DEC3-4BAD-A0BE-EBB685097DA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2249,7 +2317,7 @@
         <xdr:cNvPr id="19" name="직선 화살표 연결선 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E49A8F08-60DF-418D-8D92-E435C42894A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E49A8F08-60DF-418D-8D92-E435C42894A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2259,6 +2327,120 @@
         <a:xfrm>
           <a:off x="52055485" y="4498326"/>
           <a:ext cx="1894115" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0000FF"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>168</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>97617</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>173</xdr:col>
+      <xdr:colOff>56030</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>97617</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="직선 화살표 연결선 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B9B7B3B-4B32-4051-898C-EE6F25736D05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="45368135" y="2372411"/>
+          <a:ext cx="1360395" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="0000FF"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>172</xdr:col>
+      <xdr:colOff>259977</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95374</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>178</xdr:col>
+      <xdr:colOff>156883</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95374</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="직선 화살표 연결선 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CEEB29C9-2143-40DD-9242-A82E285F4B2E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="46641124" y="2571874"/>
+          <a:ext cx="1645024" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2580,9 +2762,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:JN47"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="EQ36" sqref="EQ36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="DX1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="FG35" sqref="FG35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2630,297 +2812,297 @@
     </row>
     <row r="6" spans="1:274" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="51"/>
-      <c r="B6" s="162">
+      <c r="B6" s="167">
         <v>9</v>
       </c>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="163"/>
-      <c r="H6" s="163"/>
-      <c r="I6" s="163"/>
-      <c r="J6" s="163"/>
-      <c r="K6" s="163"/>
-      <c r="L6" s="163"/>
-      <c r="M6" s="163"/>
-      <c r="N6" s="163"/>
-      <c r="O6" s="163"/>
-      <c r="P6" s="163"/>
-      <c r="Q6" s="163"/>
-      <c r="R6" s="163"/>
-      <c r="S6" s="163"/>
-      <c r="T6" s="163"/>
-      <c r="U6" s="163"/>
-      <c r="V6" s="163"/>
-      <c r="W6" s="163"/>
-      <c r="X6" s="163"/>
-      <c r="Y6" s="163"/>
-      <c r="Z6" s="163"/>
-      <c r="AA6" s="163"/>
-      <c r="AB6" s="163"/>
-      <c r="AC6" s="163"/>
-      <c r="AD6" s="163"/>
-      <c r="AE6" s="164"/>
-      <c r="AF6" s="159">
+      <c r="C6" s="168"/>
+      <c r="D6" s="168"/>
+      <c r="E6" s="168"/>
+      <c r="F6" s="168"/>
+      <c r="G6" s="168"/>
+      <c r="H6" s="168"/>
+      <c r="I6" s="168"/>
+      <c r="J6" s="168"/>
+      <c r="K6" s="168"/>
+      <c r="L6" s="168"/>
+      <c r="M6" s="168"/>
+      <c r="N6" s="168"/>
+      <c r="O6" s="168"/>
+      <c r="P6" s="168"/>
+      <c r="Q6" s="168"/>
+      <c r="R6" s="168"/>
+      <c r="S6" s="168"/>
+      <c r="T6" s="168"/>
+      <c r="U6" s="168"/>
+      <c r="V6" s="168"/>
+      <c r="W6" s="168"/>
+      <c r="X6" s="168"/>
+      <c r="Y6" s="168"/>
+      <c r="Z6" s="168"/>
+      <c r="AA6" s="168"/>
+      <c r="AB6" s="168"/>
+      <c r="AC6" s="168"/>
+      <c r="AD6" s="168"/>
+      <c r="AE6" s="169"/>
+      <c r="AF6" s="164">
         <v>10</v>
       </c>
-      <c r="AG6" s="159"/>
-      <c r="AH6" s="159"/>
-      <c r="AI6" s="159"/>
-      <c r="AJ6" s="159"/>
-      <c r="AK6" s="159"/>
-      <c r="AL6" s="159"/>
-      <c r="AM6" s="159"/>
-      <c r="AN6" s="159"/>
-      <c r="AO6" s="159"/>
-      <c r="AP6" s="159"/>
-      <c r="AQ6" s="159"/>
-      <c r="AR6" s="159"/>
-      <c r="AS6" s="159"/>
-      <c r="AT6" s="159"/>
-      <c r="AU6" s="159"/>
-      <c r="AV6" s="159"/>
-      <c r="AW6" s="159"/>
-      <c r="AX6" s="159"/>
-      <c r="AY6" s="159"/>
-      <c r="AZ6" s="159"/>
-      <c r="BA6" s="159"/>
-      <c r="BB6" s="159"/>
-      <c r="BC6" s="159"/>
-      <c r="BD6" s="159"/>
-      <c r="BE6" s="159"/>
-      <c r="BF6" s="159"/>
-      <c r="BG6" s="159"/>
-      <c r="BH6" s="159"/>
-      <c r="BI6" s="159"/>
-      <c r="BJ6" s="160"/>
-      <c r="BK6" s="162">
+      <c r="AG6" s="164"/>
+      <c r="AH6" s="164"/>
+      <c r="AI6" s="164"/>
+      <c r="AJ6" s="164"/>
+      <c r="AK6" s="164"/>
+      <c r="AL6" s="164"/>
+      <c r="AM6" s="164"/>
+      <c r="AN6" s="164"/>
+      <c r="AO6" s="164"/>
+      <c r="AP6" s="164"/>
+      <c r="AQ6" s="164"/>
+      <c r="AR6" s="164"/>
+      <c r="AS6" s="164"/>
+      <c r="AT6" s="164"/>
+      <c r="AU6" s="164"/>
+      <c r="AV6" s="164"/>
+      <c r="AW6" s="164"/>
+      <c r="AX6" s="164"/>
+      <c r="AY6" s="164"/>
+      <c r="AZ6" s="164"/>
+      <c r="BA6" s="164"/>
+      <c r="BB6" s="164"/>
+      <c r="BC6" s="164"/>
+      <c r="BD6" s="164"/>
+      <c r="BE6" s="164"/>
+      <c r="BF6" s="164"/>
+      <c r="BG6" s="164"/>
+      <c r="BH6" s="164"/>
+      <c r="BI6" s="164"/>
+      <c r="BJ6" s="165"/>
+      <c r="BK6" s="167">
         <v>11</v>
       </c>
-      <c r="BL6" s="163"/>
-      <c r="BM6" s="163"/>
-      <c r="BN6" s="163"/>
-      <c r="BO6" s="163"/>
-      <c r="BP6" s="163"/>
-      <c r="BQ6" s="163"/>
-      <c r="BR6" s="163"/>
-      <c r="BS6" s="163"/>
-      <c r="BT6" s="163"/>
-      <c r="BU6" s="163"/>
-      <c r="BV6" s="163"/>
-      <c r="BW6" s="163"/>
-      <c r="BX6" s="163"/>
-      <c r="BY6" s="163"/>
-      <c r="BZ6" s="163"/>
-      <c r="CA6" s="163"/>
-      <c r="CB6" s="163"/>
-      <c r="CC6" s="163"/>
-      <c r="CD6" s="163"/>
-      <c r="CE6" s="163"/>
-      <c r="CF6" s="163"/>
-      <c r="CG6" s="163"/>
-      <c r="CH6" s="163"/>
-      <c r="CI6" s="163"/>
-      <c r="CJ6" s="163"/>
-      <c r="CK6" s="163"/>
-      <c r="CL6" s="163"/>
-      <c r="CM6" s="163"/>
-      <c r="CN6" s="164"/>
-      <c r="CO6" s="159">
+      <c r="BL6" s="168"/>
+      <c r="BM6" s="168"/>
+      <c r="BN6" s="168"/>
+      <c r="BO6" s="168"/>
+      <c r="BP6" s="168"/>
+      <c r="BQ6" s="168"/>
+      <c r="BR6" s="168"/>
+      <c r="BS6" s="168"/>
+      <c r="BT6" s="168"/>
+      <c r="BU6" s="168"/>
+      <c r="BV6" s="168"/>
+      <c r="BW6" s="168"/>
+      <c r="BX6" s="168"/>
+      <c r="BY6" s="168"/>
+      <c r="BZ6" s="168"/>
+      <c r="CA6" s="168"/>
+      <c r="CB6" s="168"/>
+      <c r="CC6" s="168"/>
+      <c r="CD6" s="168"/>
+      <c r="CE6" s="168"/>
+      <c r="CF6" s="168"/>
+      <c r="CG6" s="168"/>
+      <c r="CH6" s="168"/>
+      <c r="CI6" s="168"/>
+      <c r="CJ6" s="168"/>
+      <c r="CK6" s="168"/>
+      <c r="CL6" s="168"/>
+      <c r="CM6" s="168"/>
+      <c r="CN6" s="169"/>
+      <c r="CO6" s="164">
         <v>12</v>
       </c>
-      <c r="CP6" s="159"/>
-      <c r="CQ6" s="159"/>
-      <c r="CR6" s="159"/>
-      <c r="CS6" s="159"/>
-      <c r="CT6" s="159"/>
-      <c r="CU6" s="159"/>
-      <c r="CV6" s="159"/>
-      <c r="CW6" s="159"/>
-      <c r="CX6" s="159"/>
-      <c r="CY6" s="159"/>
-      <c r="CZ6" s="159"/>
-      <c r="DA6" s="159"/>
-      <c r="DB6" s="159"/>
-      <c r="DC6" s="159"/>
-      <c r="DD6" s="159"/>
-      <c r="DE6" s="159"/>
-      <c r="DF6" s="159"/>
-      <c r="DG6" s="159"/>
-      <c r="DH6" s="159"/>
-      <c r="DI6" s="159"/>
-      <c r="DJ6" s="159"/>
-      <c r="DK6" s="159"/>
-      <c r="DL6" s="159"/>
-      <c r="DM6" s="159"/>
-      <c r="DN6" s="159"/>
-      <c r="DO6" s="159"/>
-      <c r="DP6" s="159"/>
-      <c r="DQ6" s="159"/>
-      <c r="DR6" s="159"/>
-      <c r="DS6" s="160"/>
-      <c r="DT6" s="159">
+      <c r="CP6" s="164"/>
+      <c r="CQ6" s="164"/>
+      <c r="CR6" s="164"/>
+      <c r="CS6" s="164"/>
+      <c r="CT6" s="164"/>
+      <c r="CU6" s="164"/>
+      <c r="CV6" s="164"/>
+      <c r="CW6" s="164"/>
+      <c r="CX6" s="164"/>
+      <c r="CY6" s="164"/>
+      <c r="CZ6" s="164"/>
+      <c r="DA6" s="164"/>
+      <c r="DB6" s="164"/>
+      <c r="DC6" s="164"/>
+      <c r="DD6" s="164"/>
+      <c r="DE6" s="164"/>
+      <c r="DF6" s="164"/>
+      <c r="DG6" s="164"/>
+      <c r="DH6" s="164"/>
+      <c r="DI6" s="164"/>
+      <c r="DJ6" s="164"/>
+      <c r="DK6" s="164"/>
+      <c r="DL6" s="164"/>
+      <c r="DM6" s="164"/>
+      <c r="DN6" s="164"/>
+      <c r="DO6" s="164"/>
+      <c r="DP6" s="164"/>
+      <c r="DQ6" s="164"/>
+      <c r="DR6" s="164"/>
+      <c r="DS6" s="165"/>
+      <c r="DT6" s="164">
         <v>2019.01</v>
       </c>
-      <c r="DU6" s="159"/>
-      <c r="DV6" s="159"/>
-      <c r="DW6" s="159"/>
-      <c r="DX6" s="159"/>
-      <c r="DY6" s="159"/>
-      <c r="DZ6" s="159"/>
-      <c r="EA6" s="159"/>
-      <c r="EB6" s="159"/>
-      <c r="EC6" s="159"/>
-      <c r="ED6" s="159"/>
-      <c r="EE6" s="159"/>
-      <c r="EF6" s="159"/>
-      <c r="EG6" s="159"/>
-      <c r="EH6" s="159"/>
-      <c r="EI6" s="159"/>
-      <c r="EJ6" s="159"/>
-      <c r="EK6" s="159"/>
-      <c r="EL6" s="159"/>
-      <c r="EM6" s="159"/>
-      <c r="EN6" s="159"/>
-      <c r="EO6" s="159"/>
-      <c r="EP6" s="159"/>
-      <c r="EQ6" s="159"/>
-      <c r="ER6" s="159"/>
-      <c r="ES6" s="159"/>
-      <c r="ET6" s="159"/>
-      <c r="EU6" s="159"/>
-      <c r="EV6" s="159"/>
-      <c r="EW6" s="159"/>
-      <c r="EX6" s="160"/>
-      <c r="EY6" s="161">
+      <c r="DU6" s="164"/>
+      <c r="DV6" s="164"/>
+      <c r="DW6" s="164"/>
+      <c r="DX6" s="164"/>
+      <c r="DY6" s="164"/>
+      <c r="DZ6" s="164"/>
+      <c r="EA6" s="164"/>
+      <c r="EB6" s="164"/>
+      <c r="EC6" s="164"/>
+      <c r="ED6" s="164"/>
+      <c r="EE6" s="164"/>
+      <c r="EF6" s="164"/>
+      <c r="EG6" s="164"/>
+      <c r="EH6" s="164"/>
+      <c r="EI6" s="164"/>
+      <c r="EJ6" s="164"/>
+      <c r="EK6" s="164"/>
+      <c r="EL6" s="164"/>
+      <c r="EM6" s="164"/>
+      <c r="EN6" s="164"/>
+      <c r="EO6" s="164"/>
+      <c r="EP6" s="164"/>
+      <c r="EQ6" s="164"/>
+      <c r="ER6" s="164"/>
+      <c r="ES6" s="164"/>
+      <c r="ET6" s="164"/>
+      <c r="EU6" s="164"/>
+      <c r="EV6" s="164"/>
+      <c r="EW6" s="164"/>
+      <c r="EX6" s="165"/>
+      <c r="EY6" s="166">
         <v>2019.02</v>
       </c>
-      <c r="EZ6" s="159"/>
-      <c r="FA6" s="159"/>
-      <c r="FB6" s="159"/>
-      <c r="FC6" s="159"/>
-      <c r="FD6" s="159"/>
-      <c r="FE6" s="159"/>
-      <c r="FF6" s="159"/>
-      <c r="FG6" s="159"/>
-      <c r="FH6" s="159"/>
-      <c r="FI6" s="159"/>
-      <c r="FJ6" s="159"/>
-      <c r="FK6" s="159"/>
-      <c r="FL6" s="159"/>
-      <c r="FM6" s="159"/>
-      <c r="FN6" s="159"/>
-      <c r="FO6" s="159"/>
-      <c r="FP6" s="159"/>
-      <c r="FQ6" s="159"/>
-      <c r="FR6" s="159"/>
-      <c r="FS6" s="159"/>
-      <c r="FT6" s="159"/>
-      <c r="FU6" s="159"/>
-      <c r="FV6" s="159"/>
-      <c r="FW6" s="159"/>
-      <c r="FX6" s="159"/>
-      <c r="FY6" s="159"/>
-      <c r="FZ6" s="160"/>
-      <c r="GA6" s="152">
+      <c r="EZ6" s="164"/>
+      <c r="FA6" s="164"/>
+      <c r="FB6" s="164"/>
+      <c r="FC6" s="164"/>
+      <c r="FD6" s="164"/>
+      <c r="FE6" s="164"/>
+      <c r="FF6" s="164"/>
+      <c r="FG6" s="164"/>
+      <c r="FH6" s="164"/>
+      <c r="FI6" s="164"/>
+      <c r="FJ6" s="164"/>
+      <c r="FK6" s="164"/>
+      <c r="FL6" s="164"/>
+      <c r="FM6" s="164"/>
+      <c r="FN6" s="164"/>
+      <c r="FO6" s="164"/>
+      <c r="FP6" s="164"/>
+      <c r="FQ6" s="164"/>
+      <c r="FR6" s="164"/>
+      <c r="FS6" s="164"/>
+      <c r="FT6" s="164"/>
+      <c r="FU6" s="164"/>
+      <c r="FV6" s="164"/>
+      <c r="FW6" s="164"/>
+      <c r="FX6" s="164"/>
+      <c r="FY6" s="164"/>
+      <c r="FZ6" s="165"/>
+      <c r="GA6" s="157">
         <v>3</v>
       </c>
-      <c r="GB6" s="152"/>
-      <c r="GC6" s="152"/>
-      <c r="GD6" s="152"/>
-      <c r="GE6" s="152"/>
-      <c r="GF6" s="152"/>
-      <c r="GG6" s="152"/>
-      <c r="GH6" s="152"/>
-      <c r="GI6" s="152"/>
-      <c r="GJ6" s="152"/>
-      <c r="GK6" s="152"/>
-      <c r="GL6" s="152"/>
-      <c r="GM6" s="152"/>
-      <c r="GN6" s="152"/>
-      <c r="GO6" s="152"/>
-      <c r="GP6" s="152"/>
-      <c r="GQ6" s="152"/>
-      <c r="GR6" s="152"/>
-      <c r="GS6" s="152"/>
-      <c r="GT6" s="152"/>
-      <c r="GU6" s="152"/>
-      <c r="GV6" s="152"/>
-      <c r="GW6" s="152"/>
-      <c r="GX6" s="152"/>
-      <c r="GY6" s="152"/>
-      <c r="GZ6" s="152"/>
-      <c r="HA6" s="152"/>
-      <c r="HB6" s="152"/>
-      <c r="HC6" s="152"/>
-      <c r="HD6" s="152"/>
-      <c r="HE6" s="152"/>
-      <c r="HF6" s="156">
+      <c r="GB6" s="157"/>
+      <c r="GC6" s="157"/>
+      <c r="GD6" s="157"/>
+      <c r="GE6" s="157"/>
+      <c r="GF6" s="157"/>
+      <c r="GG6" s="157"/>
+      <c r="GH6" s="157"/>
+      <c r="GI6" s="157"/>
+      <c r="GJ6" s="157"/>
+      <c r="GK6" s="157"/>
+      <c r="GL6" s="157"/>
+      <c r="GM6" s="157"/>
+      <c r="GN6" s="157"/>
+      <c r="GO6" s="157"/>
+      <c r="GP6" s="157"/>
+      <c r="GQ6" s="157"/>
+      <c r="GR6" s="157"/>
+      <c r="GS6" s="157"/>
+      <c r="GT6" s="157"/>
+      <c r="GU6" s="157"/>
+      <c r="GV6" s="157"/>
+      <c r="GW6" s="157"/>
+      <c r="GX6" s="157"/>
+      <c r="GY6" s="157"/>
+      <c r="GZ6" s="157"/>
+      <c r="HA6" s="157"/>
+      <c r="HB6" s="157"/>
+      <c r="HC6" s="157"/>
+      <c r="HD6" s="157"/>
+      <c r="HE6" s="157"/>
+      <c r="HF6" s="161">
         <v>4</v>
       </c>
-      <c r="HG6" s="157"/>
-      <c r="HH6" s="157"/>
-      <c r="HI6" s="157"/>
-      <c r="HJ6" s="157"/>
-      <c r="HK6" s="157"/>
-      <c r="HL6" s="157"/>
-      <c r="HM6" s="157"/>
-      <c r="HN6" s="157"/>
-      <c r="HO6" s="157"/>
-      <c r="HP6" s="157"/>
-      <c r="HQ6" s="157"/>
-      <c r="HR6" s="157"/>
-      <c r="HS6" s="157"/>
-      <c r="HT6" s="157"/>
-      <c r="HU6" s="157"/>
-      <c r="HV6" s="157"/>
-      <c r="HW6" s="157"/>
-      <c r="HX6" s="157"/>
-      <c r="HY6" s="157"/>
-      <c r="HZ6" s="157"/>
-      <c r="IA6" s="157"/>
-      <c r="IB6" s="157"/>
-      <c r="IC6" s="157"/>
-      <c r="ID6" s="157"/>
-      <c r="IE6" s="157"/>
-      <c r="IF6" s="157"/>
-      <c r="IG6" s="157"/>
-      <c r="IH6" s="157"/>
-      <c r="II6" s="158"/>
-      <c r="IJ6" s="151">
+      <c r="HG6" s="162"/>
+      <c r="HH6" s="162"/>
+      <c r="HI6" s="162"/>
+      <c r="HJ6" s="162"/>
+      <c r="HK6" s="162"/>
+      <c r="HL6" s="162"/>
+      <c r="HM6" s="162"/>
+      <c r="HN6" s="162"/>
+      <c r="HO6" s="162"/>
+      <c r="HP6" s="162"/>
+      <c r="HQ6" s="162"/>
+      <c r="HR6" s="162"/>
+      <c r="HS6" s="162"/>
+      <c r="HT6" s="162"/>
+      <c r="HU6" s="162"/>
+      <c r="HV6" s="162"/>
+      <c r="HW6" s="162"/>
+      <c r="HX6" s="162"/>
+      <c r="HY6" s="162"/>
+      <c r="HZ6" s="162"/>
+      <c r="IA6" s="162"/>
+      <c r="IB6" s="162"/>
+      <c r="IC6" s="162"/>
+      <c r="ID6" s="162"/>
+      <c r="IE6" s="162"/>
+      <c r="IF6" s="162"/>
+      <c r="IG6" s="162"/>
+      <c r="IH6" s="162"/>
+      <c r="II6" s="163"/>
+      <c r="IJ6" s="156">
         <v>5</v>
       </c>
-      <c r="IK6" s="152"/>
-      <c r="IL6" s="152"/>
-      <c r="IM6" s="152"/>
-      <c r="IN6" s="152"/>
-      <c r="IO6" s="152"/>
-      <c r="IP6" s="152"/>
-      <c r="IQ6" s="152"/>
-      <c r="IR6" s="152"/>
-      <c r="IS6" s="152"/>
-      <c r="IT6" s="152"/>
-      <c r="IU6" s="152"/>
-      <c r="IV6" s="152"/>
-      <c r="IW6" s="152"/>
-      <c r="IX6" s="152"/>
-      <c r="IY6" s="152"/>
-      <c r="IZ6" s="152"/>
-      <c r="JA6" s="152"/>
-      <c r="JB6" s="152"/>
-      <c r="JC6" s="152"/>
-      <c r="JD6" s="152"/>
-      <c r="JE6" s="152"/>
-      <c r="JF6" s="152"/>
-      <c r="JG6" s="152"/>
-      <c r="JH6" s="152"/>
-      <c r="JI6" s="152"/>
-      <c r="JJ6" s="152"/>
-      <c r="JK6" s="152"/>
-      <c r="JL6" s="152"/>
-      <c r="JM6" s="152"/>
-      <c r="JN6" s="153"/>
+      <c r="IK6" s="157"/>
+      <c r="IL6" s="157"/>
+      <c r="IM6" s="157"/>
+      <c r="IN6" s="157"/>
+      <c r="IO6" s="157"/>
+      <c r="IP6" s="157"/>
+      <c r="IQ6" s="157"/>
+      <c r="IR6" s="157"/>
+      <c r="IS6" s="157"/>
+      <c r="IT6" s="157"/>
+      <c r="IU6" s="157"/>
+      <c r="IV6" s="157"/>
+      <c r="IW6" s="157"/>
+      <c r="IX6" s="157"/>
+      <c r="IY6" s="157"/>
+      <c r="IZ6" s="157"/>
+      <c r="JA6" s="157"/>
+      <c r="JB6" s="157"/>
+      <c r="JC6" s="157"/>
+      <c r="JD6" s="157"/>
+      <c r="JE6" s="157"/>
+      <c r="JF6" s="157"/>
+      <c r="JG6" s="157"/>
+      <c r="JH6" s="157"/>
+      <c r="JI6" s="157"/>
+      <c r="JJ6" s="157"/>
+      <c r="JK6" s="157"/>
+      <c r="JL6" s="157"/>
+      <c r="JM6" s="157"/>
+      <c r="JN6" s="158"/>
     </row>
     <row r="7" spans="1:274" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="53"/>
@@ -3745,7 +3927,7 @@
       </c>
     </row>
     <row r="8" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="154" t="s">
+      <c r="A8" s="159" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="42"/>
@@ -3896,7 +4078,7 @@
       <c r="EK8" s="9"/>
       <c r="EL8" s="42"/>
       <c r="EM8" s="42"/>
-      <c r="EN8" s="118" t="s">
+      <c r="EN8" s="151" t="s">
         <v>15</v>
       </c>
       <c r="EO8" s="9"/>
@@ -4033,7 +4215,7 @@
       <c r="JN8" s="40"/>
     </row>
     <row r="9" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="154"/>
+      <c r="A9" s="159"/>
       <c r="B9" s="73"/>
       <c r="C9" s="74"/>
       <c r="D9" s="75"/>
@@ -4203,7 +4385,7 @@
       <c r="FF9" s="75"/>
       <c r="FG9" s="74"/>
       <c r="FH9" s="74"/>
-      <c r="FI9" s="75" t="s">
+      <c r="FI9" s="152" t="s">
         <v>19</v>
       </c>
       <c r="FJ9" s="75"/>
@@ -4321,7 +4503,7 @@
       <c r="JN9" s="7"/>
     </row>
     <row r="10" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="154"/>
+      <c r="A10" s="159"/>
       <c r="B10" s="73"/>
       <c r="C10" s="74"/>
       <c r="D10" s="75"/>
@@ -4488,7 +4670,9 @@
       <c r="FG10" s="74"/>
       <c r="FH10" s="74"/>
       <c r="FI10" s="75"/>
-      <c r="FJ10" s="75"/>
+      <c r="FJ10" s="153" t="s">
+        <v>59</v>
+      </c>
       <c r="FK10" s="75"/>
       <c r="FL10" s="75"/>
       <c r="FM10" s="75"/>
@@ -4599,7 +4783,7 @@
       <c r="JN10" s="7"/>
     </row>
     <row r="11" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="154"/>
+      <c r="A11" s="159"/>
       <c r="B11" s="73"/>
       <c r="C11" s="74"/>
       <c r="D11" s="75"/>
@@ -4877,7 +5061,7 @@
       <c r="JN11" s="7"/>
     </row>
     <row r="12" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="154"/>
+      <c r="A12" s="159"/>
       <c r="B12" s="73"/>
       <c r="C12" s="74"/>
       <c r="D12" s="75"/>
@@ -5155,7 +5339,7 @@
       <c r="JN12" s="7"/>
     </row>
     <row r="13" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="154"/>
+      <c r="A13" s="159"/>
       <c r="B13" s="73"/>
       <c r="C13" s="74"/>
       <c r="D13" s="75"/>
@@ -5431,7 +5615,7 @@
       <c r="JN13" s="7"/>
     </row>
     <row r="14" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="154"/>
+      <c r="A14" s="159"/>
       <c r="B14" s="81"/>
       <c r="C14" s="82"/>
       <c r="D14" s="83"/>
@@ -5707,7 +5891,7 @@
       <c r="JN14" s="18"/>
     </row>
     <row r="15" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="155" t="s">
+      <c r="A15" s="160" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="89"/>
@@ -5987,7 +6171,7 @@
       <c r="JN15" s="29"/>
     </row>
     <row r="16" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="154"/>
+      <c r="A16" s="159"/>
       <c r="B16" s="95"/>
       <c r="C16" s="96"/>
       <c r="D16" s="97"/>
@@ -6120,7 +6304,7 @@
       <c r="EA16" s="97"/>
       <c r="EB16" s="97"/>
       <c r="EC16" s="97"/>
-      <c r="ED16" s="100" t="s">
+      <c r="ED16" s="177" t="s">
         <v>6</v>
       </c>
       <c r="EE16" s="96"/>
@@ -6132,7 +6316,7 @@
       <c r="EK16" s="97"/>
       <c r="EL16" s="96"/>
       <c r="EM16" s="96"/>
-      <c r="EN16" s="97" t="s">
+      <c r="EN16" s="178" t="s">
         <v>11</v>
       </c>
       <c r="EO16" s="97"/>
@@ -6157,14 +6341,18 @@
       <c r="FH16" s="96"/>
       <c r="FI16" s="97"/>
       <c r="FJ16" s="97"/>
-      <c r="FK16" s="97"/>
+      <c r="FK16" s="100" t="s">
+        <v>6</v>
+      </c>
       <c r="FL16" s="97"/>
       <c r="FM16" s="97"/>
       <c r="FN16" s="96"/>
       <c r="FO16" s="96"/>
       <c r="FP16" s="97"/>
       <c r="FQ16" s="97"/>
-      <c r="FR16" s="97"/>
+      <c r="FR16" s="97" t="s">
+        <v>11</v>
+      </c>
       <c r="FS16" s="97"/>
       <c r="FT16" s="97"/>
       <c r="FU16" s="96"/>
@@ -6267,7 +6455,7 @@
       <c r="JN16" s="13"/>
     </row>
     <row r="17" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="154"/>
+      <c r="A17" s="159"/>
       <c r="B17" s="95"/>
       <c r="C17" s="96"/>
       <c r="D17" s="97"/>
@@ -6399,7 +6587,7 @@
       <c r="EA17" s="97"/>
       <c r="EB17" s="97"/>
       <c r="EC17" s="97"/>
-      <c r="ED17" s="100" t="s">
+      <c r="ED17" s="177" t="s">
         <v>10</v>
       </c>
       <c r="EE17" s="96"/>
@@ -6436,7 +6624,9 @@
       <c r="FJ17" s="97"/>
       <c r="FK17" s="97"/>
       <c r="FL17" s="97"/>
-      <c r="FM17" s="97"/>
+      <c r="FM17" s="100" t="s">
+        <v>10</v>
+      </c>
       <c r="FN17" s="96"/>
       <c r="FO17" s="96"/>
       <c r="FP17" s="97"/>
@@ -6544,7 +6734,7 @@
       <c r="JN17" s="4"/>
     </row>
     <row r="18" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="154"/>
+      <c r="A18" s="159"/>
       <c r="B18" s="95"/>
       <c r="C18" s="96"/>
       <c r="D18" s="97"/>
@@ -6821,7 +7011,7 @@
       <c r="JN18" s="4"/>
     </row>
     <row r="19" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="154"/>
+      <c r="A19" s="159"/>
       <c r="B19" s="95"/>
       <c r="C19" s="96"/>
       <c r="D19" s="97"/>
@@ -7097,7 +7287,7 @@
       <c r="JN19" s="4"/>
     </row>
     <row r="20" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="154"/>
+      <c r="A20" s="159"/>
       <c r="B20" s="95"/>
       <c r="C20" s="96"/>
       <c r="D20" s="97"/>
@@ -7373,7 +7563,7 @@
       <c r="JN20" s="4"/>
     </row>
     <row r="21" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="154"/>
+      <c r="A21" s="159"/>
       <c r="B21" s="95"/>
       <c r="C21" s="96"/>
       <c r="D21" s="97"/>
@@ -7649,7 +7839,7 @@
       <c r="JN21" s="127"/>
     </row>
     <row r="22" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="154"/>
+      <c r="A22" s="159"/>
       <c r="B22" s="102"/>
       <c r="C22" s="103"/>
       <c r="D22" s="104"/>
@@ -7925,7 +8115,7 @@
       <c r="JN22" s="25"/>
     </row>
     <row r="23" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="154" t="s">
+      <c r="A23" s="159" t="s">
         <v>29</v>
       </c>
       <c r="B23" s="108"/>
@@ -8207,7 +8397,7 @@
       <c r="JN23" s="29"/>
     </row>
     <row r="24" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="154"/>
+      <c r="A24" s="159"/>
       <c r="B24" s="95"/>
       <c r="C24" s="96"/>
       <c r="D24" s="97"/>
@@ -8485,7 +8675,7 @@
       <c r="JN24" s="4"/>
     </row>
     <row r="25" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="154"/>
+      <c r="A25" s="159"/>
       <c r="B25" s="95"/>
       <c r="C25" s="96"/>
       <c r="D25" s="97"/>
@@ -8763,7 +8953,7 @@
       <c r="JN25" s="4"/>
     </row>
     <row r="26" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="154"/>
+      <c r="A26" s="159"/>
       <c r="B26" s="95"/>
       <c r="C26" s="96"/>
       <c r="D26" s="97"/>
@@ -9047,7 +9237,7 @@
       <c r="JN26" s="4"/>
     </row>
     <row r="27" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="154"/>
+      <c r="A27" s="159"/>
       <c r="B27" s="95"/>
       <c r="C27" s="96"/>
       <c r="D27" s="97"/>
@@ -9329,7 +9519,7 @@
       <c r="JN27" s="4"/>
     </row>
     <row r="28" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="154"/>
+      <c r="A28" s="159"/>
       <c r="B28" s="95"/>
       <c r="C28" s="96"/>
       <c r="D28" s="97"/>
@@ -9607,7 +9797,7 @@
       <c r="JN28" s="4"/>
     </row>
     <row r="29" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="154"/>
+      <c r="A29" s="159"/>
       <c r="B29" s="95"/>
       <c r="C29" s="96"/>
       <c r="D29" s="97"/>
@@ -9885,7 +10075,7 @@
       <c r="JN29" s="4"/>
     </row>
     <row r="30" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="154"/>
+      <c r="A30" s="159"/>
       <c r="B30" s="102"/>
       <c r="C30" s="103"/>
       <c r="D30" s="104"/>
@@ -11432,11 +11622,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E29"/>
+  <dimension ref="B2:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11467,10 +11657,10 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="165">
+      <c r="B4" s="170">
         <v>2018.12</v>
       </c>
-      <c r="C4" s="166"/>
+      <c r="C4" s="171"/>
       <c r="D4" s="139">
         <f>SUM(D5:D13)</f>
         <v>42</v>
@@ -11478,7 +11668,7 @@
       <c r="E4" s="140"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="167">
+      <c r="B5" s="174">
         <v>12</v>
       </c>
       <c r="C5" s="143">
@@ -11492,7 +11682,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="168"/>
+      <c r="B6" s="175"/>
       <c r="C6" s="141">
         <v>17</v>
       </c>
@@ -11504,7 +11694,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="168"/>
+      <c r="B7" s="175"/>
       <c r="C7" s="141">
         <v>19</v>
       </c>
@@ -11516,7 +11706,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="168"/>
+      <c r="B8" s="175"/>
       <c r="C8" s="134">
         <v>22</v>
       </c>
@@ -11528,7 +11718,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="168"/>
+      <c r="B9" s="175"/>
       <c r="C9" s="134">
         <v>23</v>
       </c>
@@ -11540,7 +11730,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="168"/>
+      <c r="B10" s="175"/>
       <c r="C10" s="134">
         <v>25</v>
       </c>
@@ -11552,7 +11742,7 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="168"/>
+      <c r="B11" s="175"/>
       <c r="C11" s="134">
         <v>26</v>
       </c>
@@ -11564,7 +11754,7 @@
       </c>
     </row>
     <row r="12" spans="2:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="B12" s="168"/>
+      <c r="B12" s="175"/>
       <c r="C12" s="134">
         <v>29</v>
       </c>
@@ -11576,7 +11766,7 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="169"/>
+      <c r="B13" s="176"/>
       <c r="C13" s="137">
         <v>30</v>
       </c>
@@ -11588,15 +11778,15 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="165">
+      <c r="B14" s="172">
         <v>2019.01</v>
       </c>
-      <c r="C14" s="166"/>
-      <c r="D14" s="139">
+      <c r="C14" s="173"/>
+      <c r="D14" s="154">
         <f>SUM(D15:D23)</f>
         <v>34</v>
       </c>
-      <c r="E14" s="142"/>
+      <c r="E14" s="155"/>
     </row>
     <row r="15" spans="2:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B15" s="133">
@@ -11710,28 +11900,28 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="133">
+    <row r="23" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="136">
         <v>1</v>
       </c>
-      <c r="C23" s="134">
+      <c r="C23" s="137">
         <v>28</v>
       </c>
-      <c r="D23" s="135">
+      <c r="D23" s="138">
         <v>2</v>
       </c>
-      <c r="E23" s="129" t="s">
+      <c r="E23" s="130" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="165">
+      <c r="B24" s="170">
         <v>2019.01</v>
       </c>
-      <c r="C24" s="166"/>
+      <c r="C24" s="171"/>
       <c r="D24" s="139">
-        <f>SUM(D25:D35)</f>
-        <v>3</v>
+        <f>SUM(D25:D63)</f>
+        <v>12</v>
       </c>
       <c r="E24" s="142"/>
     </row>
@@ -11751,27 +11941,213 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="133"/>
-      <c r="C26" s="134"/>
-      <c r="D26" s="135"/>
-      <c r="E26" s="142"/>
+      <c r="C26" s="134">
+        <v>11</v>
+      </c>
+      <c r="D26" s="135">
+        <v>4</v>
+      </c>
+      <c r="E26" s="142" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="133"/>
-      <c r="C27" s="134"/>
-      <c r="D27" s="135"/>
-      <c r="E27" s="142"/>
+      <c r="C27" s="134">
+        <v>12</v>
+      </c>
+      <c r="D27" s="135">
+        <v>1</v>
+      </c>
+      <c r="E27" s="142" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="133"/>
-      <c r="C28" s="134"/>
-      <c r="D28" s="135"/>
-      <c r="E28" s="129"/>
+      <c r="C28" s="134">
+        <v>12</v>
+      </c>
+      <c r="D28" s="135">
+        <v>4</v>
+      </c>
+      <c r="E28" s="142" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="29" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="136"/>
-      <c r="C29" s="137"/>
-      <c r="D29" s="138"/>
-      <c r="E29" s="130"/>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="133"/>
+      <c r="C29" s="134"/>
+      <c r="D29" s="135"/>
+      <c r="E29" s="142"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="133"/>
+      <c r="C30" s="134"/>
+      <c r="D30" s="135"/>
+      <c r="E30" s="142"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="133"/>
+      <c r="C31" s="134"/>
+      <c r="D31" s="135"/>
+      <c r="E31" s="142"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="133"/>
+      <c r="C32" s="134"/>
+      <c r="D32" s="135"/>
+      <c r="E32" s="142"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="133"/>
+      <c r="C33" s="134"/>
+      <c r="D33" s="135"/>
+      <c r="E33" s="142"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="133"/>
+      <c r="C34" s="134"/>
+      <c r="D34" s="135"/>
+      <c r="E34" s="142"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="133"/>
+      <c r="C35" s="134"/>
+      <c r="D35" s="135"/>
+      <c r="E35" s="142"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="133"/>
+      <c r="C36" s="134"/>
+      <c r="D36" s="135"/>
+      <c r="E36" s="142"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B37" s="133"/>
+      <c r="C37" s="134"/>
+      <c r="D37" s="135"/>
+      <c r="E37" s="142"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38" s="133"/>
+      <c r="C38" s="134"/>
+      <c r="D38" s="135"/>
+      <c r="E38" s="142"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="133"/>
+      <c r="C39" s="134"/>
+      <c r="D39" s="135"/>
+      <c r="E39" s="142"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B40" s="133"/>
+      <c r="C40" s="134"/>
+      <c r="D40" s="135"/>
+      <c r="E40" s="142"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41" s="133"/>
+      <c r="C41" s="134"/>
+      <c r="D41" s="135"/>
+      <c r="E41" s="142"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="133"/>
+      <c r="C42" s="134"/>
+      <c r="D42" s="135"/>
+      <c r="E42" s="142"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43" s="133"/>
+      <c r="C43" s="134"/>
+      <c r="D43" s="135"/>
+      <c r="E43" s="142"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44" s="133"/>
+      <c r="C44" s="134"/>
+      <c r="D44" s="135"/>
+      <c r="E44" s="142"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B45" s="133"/>
+      <c r="C45" s="134"/>
+      <c r="D45" s="135"/>
+      <c r="E45" s="142"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46" s="133"/>
+      <c r="C46" s="134"/>
+      <c r="D46" s="135"/>
+      <c r="E46" s="142"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B47" s="133"/>
+      <c r="C47" s="134"/>
+      <c r="D47" s="135"/>
+      <c r="E47" s="142"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B48" s="133"/>
+      <c r="C48" s="134"/>
+      <c r="D48" s="135"/>
+      <c r="E48" s="142"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B49" s="133"/>
+      <c r="C49" s="134"/>
+      <c r="D49" s="135"/>
+      <c r="E49" s="142"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B50" s="133"/>
+      <c r="C50" s="134"/>
+      <c r="D50" s="135"/>
+      <c r="E50" s="142"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B51" s="133"/>
+      <c r="C51" s="134"/>
+      <c r="D51" s="135"/>
+      <c r="E51" s="142"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B52" s="133"/>
+      <c r="C52" s="134"/>
+      <c r="D52" s="135"/>
+      <c r="E52" s="142"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B53" s="133"/>
+      <c r="C53" s="134"/>
+      <c r="D53" s="135"/>
+      <c r="E53" s="142"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B54" s="133"/>
+      <c r="C54" s="134"/>
+      <c r="D54" s="135"/>
+      <c r="E54" s="142"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B55" s="133"/>
+      <c r="C55" s="134"/>
+      <c r="D55" s="135"/>
+      <c r="E55" s="142"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B56" s="133"/>
+      <c r="C56" s="134"/>
+      <c r="D56" s="135"/>
+      <c r="E56" s="129"/>
+    </row>
+    <row r="57" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="136"/>
+      <c r="C57" s="137"/>
+      <c r="D57" s="138"/>
+      <c r="E57" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
[MP data] V4.0 update
</commit_message>
<xml_diff>
--- a/Plasma Project schedule V1.0.xlsx
+++ b/Plasma Project schedule V1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="20181224" sheetId="20" r:id="rId1"/>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
   <si>
     <t>Femto Project 일정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -390,10 +390,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>◇ PCB&amp;BOM release</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>◇ 기구검토 미팅</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -447,6 +443,58 @@
   </si>
   <si>
     <t>◇ Main ME data 입수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF Gen - temp sensor 추가 / heat sink review</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF Gen - heat sink 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>◇ MP2 입고 : 5set</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>◇ PCB&amp;BOM release</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>◇ meeting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>◇ STlink 2set 전달</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>◇ DL manual 전달</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pipette MP2 DL 및 F/W review</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MP2 Booting후 바로 Off되는 issue 검증</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F/W 요청 사항 follow-up. Booting issue 해결</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Off시 LED 동기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF Gen - gerber 생성, PL 작성, 부품 구매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF Gen - PL 작성, 부품 구매</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -606,7 +654,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="53">
+  <borders count="57">
     <border>
       <left/>
       <right/>
@@ -1252,11 +1300,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1485,6 +1583,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1548,9 +1651,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1594,7 +1706,7 @@
         <xdr:cNvPr id="52" name="직선 화살표 연결선 51">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000034000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1651,7 +1763,7 @@
         <xdr:cNvPr id="15" name="직선 화살표 연결선 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1708,7 +1820,7 @@
         <xdr:cNvPr id="18" name="직선 화살표 연결선 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B9B7B3B-4B32-4051-898C-EE6F25736D05}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B9B7B3B-4B32-4051-898C-EE6F25736D05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1765,7 +1877,7 @@
         <xdr:cNvPr id="21" name="직선 화살표 연결선 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CEEB29C9-2143-40DD-9242-A82E285F4B2E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEEB29C9-2143-40DD-9242-A82E285F4B2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1822,7 +1934,7 @@
         <xdr:cNvPr id="25" name="직선 화살표 연결선 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2375196F-31DF-4BFC-AC62-19AF714F443A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2375196F-31DF-4BFC-AC62-19AF714F443A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1879,7 +1991,7 @@
         <xdr:cNvPr id="28" name="직선 화살표 연결선 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3D1266C4-6D7E-4F8B-8103-59BF7C6FE4FB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D1266C4-6D7E-4F8B-8103-59BF7C6FE4FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1936,7 +2048,7 @@
         <xdr:cNvPr id="32" name="직선 화살표 연결선 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{666CF52C-5D68-4474-8BDD-79976E036787}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{666CF52C-5D68-4474-8BDD-79976E036787}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1993,7 +2105,7 @@
         <xdr:cNvPr id="33" name="직선 화살표 연결선 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{07D67EB1-AD43-42F4-B443-3BB978B9F2AC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07D67EB1-AD43-42F4-B443-3BB978B9F2AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2050,7 +2162,7 @@
         <xdr:cNvPr id="36" name="직선 화살표 연결선 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9A732A08-4D4F-441D-9243-033ACD4A7F32}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A732A08-4D4F-441D-9243-033ACD4A7F32}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2107,7 +2219,7 @@
         <xdr:cNvPr id="38" name="직선 화살표 연결선 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3A864090-2577-47BA-8983-FFA17538A224}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A864090-2577-47BA-8983-FFA17538A224}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2164,7 +2276,7 @@
         <xdr:cNvPr id="41" name="직선 화살표 연결선 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B9CC53C-2611-4F5F-B122-A3165CFAFB90}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B9CC53C-2611-4F5F-B122-A3165CFAFB90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2221,7 +2333,7 @@
         <xdr:cNvPr id="46" name="직선 화살표 연결선 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A6CC6FD7-49CF-4859-9978-820DB474FDCC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6CC6FD7-49CF-4859-9978-820DB474FDCC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2278,7 +2390,7 @@
         <xdr:cNvPr id="14" name="직선 화살표 연결선 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A5A7DBF8-E685-466C-85D3-36D1828C9CBD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5A7DBF8-E685-466C-85D3-36D1828C9CBD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2335,7 +2447,7 @@
         <xdr:cNvPr id="16" name="직선 화살표 연결선 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8D724AD7-DEC3-4BAD-A0BE-EBB685097DA0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D724AD7-DEC3-4BAD-A0BE-EBB685097DA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2392,7 +2504,7 @@
         <xdr:cNvPr id="19" name="직선 화살표 연결선 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E49A8F08-60DF-418D-8D92-E435C42894A7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E49A8F08-60DF-418D-8D92-E435C42894A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2433,23 +2545,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>168</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:col>211</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>97617</xdr:rowOff>
+      <xdr:rowOff>116667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>173</xdr:col>
-      <xdr:colOff>56030</xdr:colOff>
+      <xdr:col>218</xdr:col>
+      <xdr:colOff>94130</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>97617</xdr:rowOff>
+      <xdr:rowOff>116667</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="17" name="직선 화살표 연결선 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B9B7B3B-4B32-4051-898C-EE6F25736D05}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B9B7B3B-4B32-4051-898C-EE6F25736D05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2457,8 +2569,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="45368135" y="2372411"/>
-          <a:ext cx="1360395" cy="0"/>
+          <a:off x="54359175" y="2364567"/>
+          <a:ext cx="1332380" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2490,23 +2602,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>172</xdr:col>
-      <xdr:colOff>259977</xdr:colOff>
+      <xdr:col>215</xdr:col>
+      <xdr:colOff>98052</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>95374</xdr:rowOff>
+      <xdr:rowOff>104899</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>178</xdr:col>
-      <xdr:colOff>156883</xdr:colOff>
+      <xdr:col>231</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>95374</xdr:rowOff>
+      <xdr:rowOff>104899</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="20" name="직선 화살표 연결선 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CEEB29C9-2143-40DD-9242-A82E285F4B2E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEEB29C9-2143-40DD-9242-A82E285F4B2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2514,8 +2626,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="46641124" y="2571874"/>
-          <a:ext cx="1645024" cy="0"/>
+          <a:off x="55095402" y="2552824"/>
+          <a:ext cx="3245223" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2837,9 +2949,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:JN47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="EO1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="GP19" sqref="GP19"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="FZ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="HR11" sqref="HR11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2887,297 +2999,297 @@
     </row>
     <row r="6" spans="1:274" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="51"/>
-      <c r="B6" s="169">
+      <c r="B6" s="174">
         <v>9</v>
       </c>
-      <c r="C6" s="170"/>
-      <c r="D6" s="170"/>
-      <c r="E6" s="170"/>
-      <c r="F6" s="170"/>
-      <c r="G6" s="170"/>
-      <c r="H6" s="170"/>
-      <c r="I6" s="170"/>
-      <c r="J6" s="170"/>
-      <c r="K6" s="170"/>
-      <c r="L6" s="170"/>
-      <c r="M6" s="170"/>
-      <c r="N6" s="170"/>
-      <c r="O6" s="170"/>
-      <c r="P6" s="170"/>
-      <c r="Q6" s="170"/>
-      <c r="R6" s="170"/>
-      <c r="S6" s="170"/>
-      <c r="T6" s="170"/>
-      <c r="U6" s="170"/>
-      <c r="V6" s="170"/>
-      <c r="W6" s="170"/>
-      <c r="X6" s="170"/>
-      <c r="Y6" s="170"/>
-      <c r="Z6" s="170"/>
-      <c r="AA6" s="170"/>
-      <c r="AB6" s="170"/>
-      <c r="AC6" s="170"/>
-      <c r="AD6" s="170"/>
-      <c r="AE6" s="171"/>
-      <c r="AF6" s="166">
+      <c r="C6" s="175"/>
+      <c r="D6" s="175"/>
+      <c r="E6" s="175"/>
+      <c r="F6" s="175"/>
+      <c r="G6" s="175"/>
+      <c r="H6" s="175"/>
+      <c r="I6" s="175"/>
+      <c r="J6" s="175"/>
+      <c r="K6" s="175"/>
+      <c r="L6" s="175"/>
+      <c r="M6" s="175"/>
+      <c r="N6" s="175"/>
+      <c r="O6" s="175"/>
+      <c r="P6" s="175"/>
+      <c r="Q6" s="175"/>
+      <c r="R6" s="175"/>
+      <c r="S6" s="175"/>
+      <c r="T6" s="175"/>
+      <c r="U6" s="175"/>
+      <c r="V6" s="175"/>
+      <c r="W6" s="175"/>
+      <c r="X6" s="175"/>
+      <c r="Y6" s="175"/>
+      <c r="Z6" s="175"/>
+      <c r="AA6" s="175"/>
+      <c r="AB6" s="175"/>
+      <c r="AC6" s="175"/>
+      <c r="AD6" s="175"/>
+      <c r="AE6" s="176"/>
+      <c r="AF6" s="171">
         <v>10</v>
       </c>
-      <c r="AG6" s="166"/>
-      <c r="AH6" s="166"/>
-      <c r="AI6" s="166"/>
-      <c r="AJ6" s="166"/>
-      <c r="AK6" s="166"/>
-      <c r="AL6" s="166"/>
-      <c r="AM6" s="166"/>
-      <c r="AN6" s="166"/>
-      <c r="AO6" s="166"/>
-      <c r="AP6" s="166"/>
-      <c r="AQ6" s="166"/>
-      <c r="AR6" s="166"/>
-      <c r="AS6" s="166"/>
-      <c r="AT6" s="166"/>
-      <c r="AU6" s="166"/>
-      <c r="AV6" s="166"/>
-      <c r="AW6" s="166"/>
-      <c r="AX6" s="166"/>
-      <c r="AY6" s="166"/>
-      <c r="AZ6" s="166"/>
-      <c r="BA6" s="166"/>
-      <c r="BB6" s="166"/>
-      <c r="BC6" s="166"/>
-      <c r="BD6" s="166"/>
-      <c r="BE6" s="166"/>
-      <c r="BF6" s="166"/>
-      <c r="BG6" s="166"/>
-      <c r="BH6" s="166"/>
-      <c r="BI6" s="166"/>
-      <c r="BJ6" s="167"/>
-      <c r="BK6" s="169">
+      <c r="AG6" s="171"/>
+      <c r="AH6" s="171"/>
+      <c r="AI6" s="171"/>
+      <c r="AJ6" s="171"/>
+      <c r="AK6" s="171"/>
+      <c r="AL6" s="171"/>
+      <c r="AM6" s="171"/>
+      <c r="AN6" s="171"/>
+      <c r="AO6" s="171"/>
+      <c r="AP6" s="171"/>
+      <c r="AQ6" s="171"/>
+      <c r="AR6" s="171"/>
+      <c r="AS6" s="171"/>
+      <c r="AT6" s="171"/>
+      <c r="AU6" s="171"/>
+      <c r="AV6" s="171"/>
+      <c r="AW6" s="171"/>
+      <c r="AX6" s="171"/>
+      <c r="AY6" s="171"/>
+      <c r="AZ6" s="171"/>
+      <c r="BA6" s="171"/>
+      <c r="BB6" s="171"/>
+      <c r="BC6" s="171"/>
+      <c r="BD6" s="171"/>
+      <c r="BE6" s="171"/>
+      <c r="BF6" s="171"/>
+      <c r="BG6" s="171"/>
+      <c r="BH6" s="171"/>
+      <c r="BI6" s="171"/>
+      <c r="BJ6" s="172"/>
+      <c r="BK6" s="174">
         <v>11</v>
       </c>
-      <c r="BL6" s="170"/>
-      <c r="BM6" s="170"/>
-      <c r="BN6" s="170"/>
-      <c r="BO6" s="170"/>
-      <c r="BP6" s="170"/>
-      <c r="BQ6" s="170"/>
-      <c r="BR6" s="170"/>
-      <c r="BS6" s="170"/>
-      <c r="BT6" s="170"/>
-      <c r="BU6" s="170"/>
-      <c r="BV6" s="170"/>
-      <c r="BW6" s="170"/>
-      <c r="BX6" s="170"/>
-      <c r="BY6" s="170"/>
-      <c r="BZ6" s="170"/>
-      <c r="CA6" s="170"/>
-      <c r="CB6" s="170"/>
-      <c r="CC6" s="170"/>
-      <c r="CD6" s="170"/>
-      <c r="CE6" s="170"/>
-      <c r="CF6" s="170"/>
-      <c r="CG6" s="170"/>
-      <c r="CH6" s="170"/>
-      <c r="CI6" s="170"/>
-      <c r="CJ6" s="170"/>
-      <c r="CK6" s="170"/>
-      <c r="CL6" s="170"/>
-      <c r="CM6" s="170"/>
-      <c r="CN6" s="171"/>
-      <c r="CO6" s="166">
+      <c r="BL6" s="175"/>
+      <c r="BM6" s="175"/>
+      <c r="BN6" s="175"/>
+      <c r="BO6" s="175"/>
+      <c r="BP6" s="175"/>
+      <c r="BQ6" s="175"/>
+      <c r="BR6" s="175"/>
+      <c r="BS6" s="175"/>
+      <c r="BT6" s="175"/>
+      <c r="BU6" s="175"/>
+      <c r="BV6" s="175"/>
+      <c r="BW6" s="175"/>
+      <c r="BX6" s="175"/>
+      <c r="BY6" s="175"/>
+      <c r="BZ6" s="175"/>
+      <c r="CA6" s="175"/>
+      <c r="CB6" s="175"/>
+      <c r="CC6" s="175"/>
+      <c r="CD6" s="175"/>
+      <c r="CE6" s="175"/>
+      <c r="CF6" s="175"/>
+      <c r="CG6" s="175"/>
+      <c r="CH6" s="175"/>
+      <c r="CI6" s="175"/>
+      <c r="CJ6" s="175"/>
+      <c r="CK6" s="175"/>
+      <c r="CL6" s="175"/>
+      <c r="CM6" s="175"/>
+      <c r="CN6" s="176"/>
+      <c r="CO6" s="171">
         <v>12</v>
       </c>
-      <c r="CP6" s="166"/>
-      <c r="CQ6" s="166"/>
-      <c r="CR6" s="166"/>
-      <c r="CS6" s="166"/>
-      <c r="CT6" s="166"/>
-      <c r="CU6" s="166"/>
-      <c r="CV6" s="166"/>
-      <c r="CW6" s="166"/>
-      <c r="CX6" s="166"/>
-      <c r="CY6" s="166"/>
-      <c r="CZ6" s="166"/>
-      <c r="DA6" s="166"/>
-      <c r="DB6" s="166"/>
-      <c r="DC6" s="166"/>
-      <c r="DD6" s="166"/>
-      <c r="DE6" s="166"/>
-      <c r="DF6" s="166"/>
-      <c r="DG6" s="166"/>
-      <c r="DH6" s="166"/>
-      <c r="DI6" s="166"/>
-      <c r="DJ6" s="166"/>
-      <c r="DK6" s="166"/>
-      <c r="DL6" s="166"/>
-      <c r="DM6" s="166"/>
-      <c r="DN6" s="166"/>
-      <c r="DO6" s="166"/>
-      <c r="DP6" s="166"/>
-      <c r="DQ6" s="166"/>
-      <c r="DR6" s="166"/>
-      <c r="DS6" s="167"/>
-      <c r="DT6" s="166">
+      <c r="CP6" s="171"/>
+      <c r="CQ6" s="171"/>
+      <c r="CR6" s="171"/>
+      <c r="CS6" s="171"/>
+      <c r="CT6" s="171"/>
+      <c r="CU6" s="171"/>
+      <c r="CV6" s="171"/>
+      <c r="CW6" s="171"/>
+      <c r="CX6" s="171"/>
+      <c r="CY6" s="171"/>
+      <c r="CZ6" s="171"/>
+      <c r="DA6" s="171"/>
+      <c r="DB6" s="171"/>
+      <c r="DC6" s="171"/>
+      <c r="DD6" s="171"/>
+      <c r="DE6" s="171"/>
+      <c r="DF6" s="171"/>
+      <c r="DG6" s="171"/>
+      <c r="DH6" s="171"/>
+      <c r="DI6" s="171"/>
+      <c r="DJ6" s="171"/>
+      <c r="DK6" s="171"/>
+      <c r="DL6" s="171"/>
+      <c r="DM6" s="171"/>
+      <c r="DN6" s="171"/>
+      <c r="DO6" s="171"/>
+      <c r="DP6" s="171"/>
+      <c r="DQ6" s="171"/>
+      <c r="DR6" s="171"/>
+      <c r="DS6" s="172"/>
+      <c r="DT6" s="171">
         <v>2019.01</v>
       </c>
-      <c r="DU6" s="166"/>
-      <c r="DV6" s="166"/>
-      <c r="DW6" s="166"/>
-      <c r="DX6" s="166"/>
-      <c r="DY6" s="166"/>
-      <c r="DZ6" s="166"/>
-      <c r="EA6" s="166"/>
-      <c r="EB6" s="166"/>
-      <c r="EC6" s="166"/>
-      <c r="ED6" s="166"/>
-      <c r="EE6" s="166"/>
-      <c r="EF6" s="166"/>
-      <c r="EG6" s="166"/>
-      <c r="EH6" s="166"/>
-      <c r="EI6" s="166"/>
-      <c r="EJ6" s="166"/>
-      <c r="EK6" s="166"/>
-      <c r="EL6" s="166"/>
-      <c r="EM6" s="166"/>
-      <c r="EN6" s="166"/>
-      <c r="EO6" s="166"/>
-      <c r="EP6" s="166"/>
-      <c r="EQ6" s="166"/>
-      <c r="ER6" s="166"/>
-      <c r="ES6" s="166"/>
-      <c r="ET6" s="166"/>
-      <c r="EU6" s="166"/>
-      <c r="EV6" s="166"/>
-      <c r="EW6" s="166"/>
-      <c r="EX6" s="167"/>
-      <c r="EY6" s="168">
+      <c r="DU6" s="171"/>
+      <c r="DV6" s="171"/>
+      <c r="DW6" s="171"/>
+      <c r="DX6" s="171"/>
+      <c r="DY6" s="171"/>
+      <c r="DZ6" s="171"/>
+      <c r="EA6" s="171"/>
+      <c r="EB6" s="171"/>
+      <c r="EC6" s="171"/>
+      <c r="ED6" s="171"/>
+      <c r="EE6" s="171"/>
+      <c r="EF6" s="171"/>
+      <c r="EG6" s="171"/>
+      <c r="EH6" s="171"/>
+      <c r="EI6" s="171"/>
+      <c r="EJ6" s="171"/>
+      <c r="EK6" s="171"/>
+      <c r="EL6" s="171"/>
+      <c r="EM6" s="171"/>
+      <c r="EN6" s="171"/>
+      <c r="EO6" s="171"/>
+      <c r="EP6" s="171"/>
+      <c r="EQ6" s="171"/>
+      <c r="ER6" s="171"/>
+      <c r="ES6" s="171"/>
+      <c r="ET6" s="171"/>
+      <c r="EU6" s="171"/>
+      <c r="EV6" s="171"/>
+      <c r="EW6" s="171"/>
+      <c r="EX6" s="172"/>
+      <c r="EY6" s="173">
         <v>2019.02</v>
       </c>
-      <c r="EZ6" s="166"/>
-      <c r="FA6" s="166"/>
-      <c r="FB6" s="166"/>
-      <c r="FC6" s="166"/>
-      <c r="FD6" s="166"/>
-      <c r="FE6" s="166"/>
-      <c r="FF6" s="166"/>
-      <c r="FG6" s="166"/>
-      <c r="FH6" s="166"/>
-      <c r="FI6" s="166"/>
-      <c r="FJ6" s="166"/>
-      <c r="FK6" s="166"/>
-      <c r="FL6" s="166"/>
-      <c r="FM6" s="166"/>
-      <c r="FN6" s="166"/>
-      <c r="FO6" s="166"/>
-      <c r="FP6" s="166"/>
-      <c r="FQ6" s="166"/>
-      <c r="FR6" s="166"/>
-      <c r="FS6" s="166"/>
-      <c r="FT6" s="166"/>
-      <c r="FU6" s="166"/>
-      <c r="FV6" s="166"/>
-      <c r="FW6" s="166"/>
-      <c r="FX6" s="166"/>
-      <c r="FY6" s="166"/>
-      <c r="FZ6" s="167"/>
-      <c r="GA6" s="159">
+      <c r="EZ6" s="171"/>
+      <c r="FA6" s="171"/>
+      <c r="FB6" s="171"/>
+      <c r="FC6" s="171"/>
+      <c r="FD6" s="171"/>
+      <c r="FE6" s="171"/>
+      <c r="FF6" s="171"/>
+      <c r="FG6" s="171"/>
+      <c r="FH6" s="171"/>
+      <c r="FI6" s="171"/>
+      <c r="FJ6" s="171"/>
+      <c r="FK6" s="171"/>
+      <c r="FL6" s="171"/>
+      <c r="FM6" s="171"/>
+      <c r="FN6" s="171"/>
+      <c r="FO6" s="171"/>
+      <c r="FP6" s="171"/>
+      <c r="FQ6" s="171"/>
+      <c r="FR6" s="171"/>
+      <c r="FS6" s="171"/>
+      <c r="FT6" s="171"/>
+      <c r="FU6" s="171"/>
+      <c r="FV6" s="171"/>
+      <c r="FW6" s="171"/>
+      <c r="FX6" s="171"/>
+      <c r="FY6" s="171"/>
+      <c r="FZ6" s="172"/>
+      <c r="GA6" s="164">
         <v>3</v>
       </c>
-      <c r="GB6" s="159"/>
-      <c r="GC6" s="159"/>
-      <c r="GD6" s="159"/>
-      <c r="GE6" s="159"/>
-      <c r="GF6" s="159"/>
-      <c r="GG6" s="159"/>
-      <c r="GH6" s="159"/>
-      <c r="GI6" s="159"/>
-      <c r="GJ6" s="159"/>
-      <c r="GK6" s="159"/>
-      <c r="GL6" s="159"/>
-      <c r="GM6" s="159"/>
-      <c r="GN6" s="159"/>
-      <c r="GO6" s="159"/>
-      <c r="GP6" s="159"/>
-      <c r="GQ6" s="159"/>
-      <c r="GR6" s="159"/>
-      <c r="GS6" s="159"/>
-      <c r="GT6" s="159"/>
-      <c r="GU6" s="159"/>
-      <c r="GV6" s="159"/>
-      <c r="GW6" s="159"/>
-      <c r="GX6" s="159"/>
-      <c r="GY6" s="159"/>
-      <c r="GZ6" s="159"/>
-      <c r="HA6" s="159"/>
-      <c r="HB6" s="159"/>
-      <c r="HC6" s="159"/>
-      <c r="HD6" s="159"/>
-      <c r="HE6" s="159"/>
-      <c r="HF6" s="163">
+      <c r="GB6" s="164"/>
+      <c r="GC6" s="164"/>
+      <c r="GD6" s="164"/>
+      <c r="GE6" s="164"/>
+      <c r="GF6" s="164"/>
+      <c r="GG6" s="164"/>
+      <c r="GH6" s="164"/>
+      <c r="GI6" s="164"/>
+      <c r="GJ6" s="164"/>
+      <c r="GK6" s="164"/>
+      <c r="GL6" s="164"/>
+      <c r="GM6" s="164"/>
+      <c r="GN6" s="164"/>
+      <c r="GO6" s="164"/>
+      <c r="GP6" s="164"/>
+      <c r="GQ6" s="164"/>
+      <c r="GR6" s="164"/>
+      <c r="GS6" s="164"/>
+      <c r="GT6" s="164"/>
+      <c r="GU6" s="164"/>
+      <c r="GV6" s="164"/>
+      <c r="GW6" s="164"/>
+      <c r="GX6" s="164"/>
+      <c r="GY6" s="164"/>
+      <c r="GZ6" s="164"/>
+      <c r="HA6" s="164"/>
+      <c r="HB6" s="164"/>
+      <c r="HC6" s="164"/>
+      <c r="HD6" s="164"/>
+      <c r="HE6" s="164"/>
+      <c r="HF6" s="168">
         <v>4</v>
       </c>
-      <c r="HG6" s="164"/>
-      <c r="HH6" s="164"/>
-      <c r="HI6" s="164"/>
-      <c r="HJ6" s="164"/>
-      <c r="HK6" s="164"/>
-      <c r="HL6" s="164"/>
-      <c r="HM6" s="164"/>
-      <c r="HN6" s="164"/>
-      <c r="HO6" s="164"/>
-      <c r="HP6" s="164"/>
-      <c r="HQ6" s="164"/>
-      <c r="HR6" s="164"/>
-      <c r="HS6" s="164"/>
-      <c r="HT6" s="164"/>
-      <c r="HU6" s="164"/>
-      <c r="HV6" s="164"/>
-      <c r="HW6" s="164"/>
-      <c r="HX6" s="164"/>
-      <c r="HY6" s="164"/>
-      <c r="HZ6" s="164"/>
-      <c r="IA6" s="164"/>
-      <c r="IB6" s="164"/>
-      <c r="IC6" s="164"/>
-      <c r="ID6" s="164"/>
-      <c r="IE6" s="164"/>
-      <c r="IF6" s="164"/>
-      <c r="IG6" s="164"/>
-      <c r="IH6" s="164"/>
-      <c r="II6" s="165"/>
-      <c r="IJ6" s="158">
+      <c r="HG6" s="169"/>
+      <c r="HH6" s="169"/>
+      <c r="HI6" s="169"/>
+      <c r="HJ6" s="169"/>
+      <c r="HK6" s="169"/>
+      <c r="HL6" s="169"/>
+      <c r="HM6" s="169"/>
+      <c r="HN6" s="169"/>
+      <c r="HO6" s="169"/>
+      <c r="HP6" s="169"/>
+      <c r="HQ6" s="169"/>
+      <c r="HR6" s="169"/>
+      <c r="HS6" s="169"/>
+      <c r="HT6" s="169"/>
+      <c r="HU6" s="169"/>
+      <c r="HV6" s="169"/>
+      <c r="HW6" s="169"/>
+      <c r="HX6" s="169"/>
+      <c r="HY6" s="169"/>
+      <c r="HZ6" s="169"/>
+      <c r="IA6" s="169"/>
+      <c r="IB6" s="169"/>
+      <c r="IC6" s="169"/>
+      <c r="ID6" s="169"/>
+      <c r="IE6" s="169"/>
+      <c r="IF6" s="169"/>
+      <c r="IG6" s="169"/>
+      <c r="IH6" s="169"/>
+      <c r="II6" s="170"/>
+      <c r="IJ6" s="163">
         <v>5</v>
       </c>
-      <c r="IK6" s="159"/>
-      <c r="IL6" s="159"/>
-      <c r="IM6" s="159"/>
-      <c r="IN6" s="159"/>
-      <c r="IO6" s="159"/>
-      <c r="IP6" s="159"/>
-      <c r="IQ6" s="159"/>
-      <c r="IR6" s="159"/>
-      <c r="IS6" s="159"/>
-      <c r="IT6" s="159"/>
-      <c r="IU6" s="159"/>
-      <c r="IV6" s="159"/>
-      <c r="IW6" s="159"/>
-      <c r="IX6" s="159"/>
-      <c r="IY6" s="159"/>
-      <c r="IZ6" s="159"/>
-      <c r="JA6" s="159"/>
-      <c r="JB6" s="159"/>
-      <c r="JC6" s="159"/>
-      <c r="JD6" s="159"/>
-      <c r="JE6" s="159"/>
-      <c r="JF6" s="159"/>
-      <c r="JG6" s="159"/>
-      <c r="JH6" s="159"/>
-      <c r="JI6" s="159"/>
-      <c r="JJ6" s="159"/>
-      <c r="JK6" s="159"/>
-      <c r="JL6" s="159"/>
-      <c r="JM6" s="159"/>
-      <c r="JN6" s="160"/>
+      <c r="IK6" s="164"/>
+      <c r="IL6" s="164"/>
+      <c r="IM6" s="164"/>
+      <c r="IN6" s="164"/>
+      <c r="IO6" s="164"/>
+      <c r="IP6" s="164"/>
+      <c r="IQ6" s="164"/>
+      <c r="IR6" s="164"/>
+      <c r="IS6" s="164"/>
+      <c r="IT6" s="164"/>
+      <c r="IU6" s="164"/>
+      <c r="IV6" s="164"/>
+      <c r="IW6" s="164"/>
+      <c r="IX6" s="164"/>
+      <c r="IY6" s="164"/>
+      <c r="IZ6" s="164"/>
+      <c r="JA6" s="164"/>
+      <c r="JB6" s="164"/>
+      <c r="JC6" s="164"/>
+      <c r="JD6" s="164"/>
+      <c r="JE6" s="164"/>
+      <c r="JF6" s="164"/>
+      <c r="JG6" s="164"/>
+      <c r="JH6" s="164"/>
+      <c r="JI6" s="164"/>
+      <c r="JJ6" s="164"/>
+      <c r="JK6" s="164"/>
+      <c r="JL6" s="164"/>
+      <c r="JM6" s="164"/>
+      <c r="JN6" s="165"/>
     </row>
     <row r="7" spans="1:274" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="53"/>
@@ -4002,7 +4114,7 @@
       </c>
     </row>
     <row r="8" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="161" t="s">
+      <c r="A8" s="166" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="42"/>
@@ -4227,7 +4339,9 @@
       <c r="HC8" s="8"/>
       <c r="HD8" s="42"/>
       <c r="HE8" s="10"/>
-      <c r="HF8" s="21"/>
+      <c r="HF8" s="162" t="s">
+        <v>84</v>
+      </c>
       <c r="HG8" s="8"/>
       <c r="HH8" s="8"/>
       <c r="HI8" s="8"/>
@@ -4290,7 +4404,7 @@
       <c r="JN8" s="40"/>
     </row>
     <row r="9" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="161"/>
+      <c r="A9" s="166"/>
       <c r="B9" s="73"/>
       <c r="C9" s="74"/>
       <c r="D9" s="75"/>
@@ -4582,7 +4696,7 @@
       <c r="JN9" s="7"/>
     </row>
     <row r="10" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="161"/>
+      <c r="A10" s="166"/>
       <c r="B10" s="73"/>
       <c r="C10" s="74"/>
       <c r="D10" s="75"/>
@@ -4768,7 +4882,7 @@
       <c r="FX10" s="75"/>
       <c r="FY10" s="75"/>
       <c r="FZ10" s="75" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="GA10" s="33"/>
       <c r="GB10" s="6"/>
@@ -4781,7 +4895,7 @@
       <c r="GI10" s="6"/>
       <c r="GJ10" s="6"/>
       <c r="GK10" s="75" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="GL10" s="5"/>
       <c r="GM10" s="5"/>
@@ -4866,7 +4980,7 @@
       <c r="JN10" s="7"/>
     </row>
     <row r="11" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="161"/>
+      <c r="A11" s="166"/>
       <c r="B11" s="73"/>
       <c r="C11" s="74"/>
       <c r="D11" s="75"/>
@@ -5064,7 +5178,7 @@
       <c r="GL11" s="5"/>
       <c r="GM11" s="5"/>
       <c r="GN11" s="117" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="GO11" s="5"/>
       <c r="GP11" s="6"/>
@@ -5083,7 +5197,9 @@
       <c r="HC11" s="5"/>
       <c r="HD11" s="6"/>
       <c r="HE11" s="6"/>
-      <c r="HF11" s="16"/>
+      <c r="HF11" s="117" t="s">
+        <v>82</v>
+      </c>
       <c r="HG11" s="5"/>
       <c r="HH11" s="5"/>
       <c r="HI11" s="5"/>
@@ -5146,7 +5262,7 @@
       <c r="JN11" s="7"/>
     </row>
     <row r="12" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="161"/>
+      <c r="A12" s="166"/>
       <c r="B12" s="73"/>
       <c r="C12" s="74"/>
       <c r="D12" s="75"/>
@@ -5332,8 +5448,8 @@
       <c r="FZ12" s="79"/>
       <c r="GA12" s="33"/>
       <c r="GB12" s="6"/>
-      <c r="GC12" s="179" t="s">
-        <v>78</v>
+      <c r="GC12" s="158" t="s">
+        <v>77</v>
       </c>
       <c r="GD12" s="5"/>
       <c r="GE12" s="5"/>
@@ -5347,8 +5463,8 @@
       <c r="GM12" s="5"/>
       <c r="GN12" s="5"/>
       <c r="GO12" s="5"/>
-      <c r="GP12" s="181" t="s">
-        <v>79</v>
+      <c r="GP12" s="160" t="s">
+        <v>78</v>
       </c>
       <c r="GQ12" s="6"/>
       <c r="GR12" s="5"/>
@@ -5365,7 +5481,9 @@
       <c r="HC12" s="5"/>
       <c r="HD12" s="6"/>
       <c r="HE12" s="6"/>
-      <c r="HF12" s="16"/>
+      <c r="HF12" s="117" t="s">
+        <v>85</v>
+      </c>
       <c r="HG12" s="5"/>
       <c r="HH12" s="5"/>
       <c r="HI12" s="5"/>
@@ -5428,7 +5546,7 @@
       <c r="JN12" s="7"/>
     </row>
     <row r="13" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="161"/>
+      <c r="A13" s="166"/>
       <c r="B13" s="73"/>
       <c r="C13" s="74"/>
       <c r="D13" s="75"/>
@@ -5612,8 +5730,8 @@
       <c r="FZ13" s="79"/>
       <c r="GA13" s="33"/>
       <c r="GB13" s="6"/>
-      <c r="GC13" s="179" t="s">
-        <v>76</v>
+      <c r="GC13" s="158" t="s">
+        <v>75</v>
       </c>
       <c r="GD13" s="5"/>
       <c r="GE13" s="5"/>
@@ -5643,7 +5761,9 @@
       <c r="HC13" s="5"/>
       <c r="HD13" s="6"/>
       <c r="HE13" s="6"/>
-      <c r="HF13" s="16"/>
+      <c r="HF13" s="161" t="s">
+        <v>86</v>
+      </c>
       <c r="HG13" s="5"/>
       <c r="HH13" s="5"/>
       <c r="HI13" s="5"/>
@@ -5706,7 +5826,7 @@
       <c r="JN13" s="7"/>
     </row>
     <row r="14" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="161"/>
+      <c r="A14" s="166"/>
       <c r="B14" s="81"/>
       <c r="C14" s="82"/>
       <c r="D14" s="83"/>
@@ -5893,8 +6013,8 @@
       <c r="GC14" s="15"/>
       <c r="GD14" s="14"/>
       <c r="GE14" s="14"/>
-      <c r="GF14" s="180" t="s">
-        <v>77</v>
+      <c r="GF14" s="159" t="s">
+        <v>76</v>
       </c>
       <c r="GG14" s="14"/>
       <c r="GH14" s="14"/>
@@ -5984,7 +6104,7 @@
       <c r="JN14" s="18"/>
     </row>
     <row r="15" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="162" t="s">
+      <c r="A15" s="167" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="89"/>
@@ -6264,7 +6384,7 @@
       <c r="JN15" s="29"/>
     </row>
     <row r="16" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="161"/>
+      <c r="A16" s="166"/>
       <c r="B16" s="95"/>
       <c r="C16" s="96"/>
       <c r="D16" s="97"/>
@@ -6480,7 +6600,9 @@
       <c r="GX16" s="12"/>
       <c r="GY16" s="11"/>
       <c r="GZ16" s="11"/>
-      <c r="HA16" s="11"/>
+      <c r="HA16" s="100" t="s">
+        <v>6</v>
+      </c>
       <c r="HB16" s="11"/>
       <c r="HC16" s="11"/>
       <c r="HD16" s="12"/>
@@ -6497,7 +6619,9 @@
       <c r="HO16" s="11"/>
       <c r="HP16" s="11"/>
       <c r="HQ16" s="11"/>
-      <c r="HR16" s="12"/>
+      <c r="HR16" s="97" t="s">
+        <v>11</v>
+      </c>
       <c r="HS16" s="12"/>
       <c r="HT16" s="11"/>
       <c r="HU16" s="11"/>
@@ -6548,7 +6672,7 @@
       <c r="JN16" s="13"/>
     </row>
     <row r="17" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="161"/>
+      <c r="A17" s="166"/>
       <c r="B17" s="95"/>
       <c r="C17" s="96"/>
       <c r="D17" s="97"/>
@@ -6759,7 +6883,9 @@
       <c r="GX17" s="1"/>
       <c r="GY17" s="2"/>
       <c r="GZ17" s="2"/>
-      <c r="HA17" s="2"/>
+      <c r="HA17" s="100" t="s">
+        <v>10</v>
+      </c>
       <c r="HB17" s="2"/>
       <c r="HC17" s="2"/>
       <c r="HD17" s="1"/>
@@ -6827,7 +6953,7 @@
       <c r="JN17" s="4"/>
     </row>
     <row r="18" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="161"/>
+      <c r="A18" s="166"/>
       <c r="B18" s="95"/>
       <c r="C18" s="96"/>
       <c r="D18" s="97"/>
@@ -7104,7 +7230,7 @@
       <c r="JN18" s="4"/>
     </row>
     <row r="19" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="161"/>
+      <c r="A19" s="166"/>
       <c r="B19" s="95"/>
       <c r="C19" s="96"/>
       <c r="D19" s="97"/>
@@ -7380,7 +7506,7 @@
       <c r="JN19" s="4"/>
     </row>
     <row r="20" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="161"/>
+      <c r="A20" s="166"/>
       <c r="B20" s="95"/>
       <c r="C20" s="96"/>
       <c r="D20" s="97"/>
@@ -7656,7 +7782,7 @@
       <c r="JN20" s="4"/>
     </row>
     <row r="21" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="161"/>
+      <c r="A21" s="166"/>
       <c r="B21" s="95"/>
       <c r="C21" s="96"/>
       <c r="D21" s="97"/>
@@ -7932,7 +8058,7 @@
       <c r="JN21" s="127"/>
     </row>
     <row r="22" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="161"/>
+      <c r="A22" s="166"/>
       <c r="B22" s="102"/>
       <c r="C22" s="103"/>
       <c r="D22" s="104"/>
@@ -8208,7 +8334,7 @@
       <c r="JN22" s="25"/>
     </row>
     <row r="23" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="161" t="s">
+      <c r="A23" s="166" t="s">
         <v>29</v>
       </c>
       <c r="B23" s="108"/>
@@ -8490,7 +8616,7 @@
       <c r="JN23" s="29"/>
     </row>
     <row r="24" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="161"/>
+      <c r="A24" s="166"/>
       <c r="B24" s="95"/>
       <c r="C24" s="96"/>
       <c r="D24" s="97"/>
@@ -8768,7 +8894,7 @@
       <c r="JN24" s="4"/>
     </row>
     <row r="25" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="161"/>
+      <c r="A25" s="166"/>
       <c r="B25" s="95"/>
       <c r="C25" s="96"/>
       <c r="D25" s="97"/>
@@ -9046,7 +9172,7 @@
       <c r="JN25" s="4"/>
     </row>
     <row r="26" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="161"/>
+      <c r="A26" s="166"/>
       <c r="B26" s="95"/>
       <c r="C26" s="96"/>
       <c r="D26" s="97"/>
@@ -9330,7 +9456,7 @@
       <c r="JN26" s="4"/>
     </row>
     <row r="27" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="161"/>
+      <c r="A27" s="166"/>
       <c r="B27" s="95"/>
       <c r="C27" s="96"/>
       <c r="D27" s="97"/>
@@ -9612,7 +9738,7 @@
       <c r="JN27" s="4"/>
     </row>
     <row r="28" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="161"/>
+      <c r="A28" s="166"/>
       <c r="B28" s="95"/>
       <c r="C28" s="96"/>
       <c r="D28" s="97"/>
@@ -9890,7 +10016,7 @@
       <c r="JN28" s="4"/>
     </row>
     <row r="29" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="161"/>
+      <c r="A29" s="166"/>
       <c r="B29" s="95"/>
       <c r="C29" s="96"/>
       <c r="D29" s="97"/>
@@ -10168,7 +10294,7 @@
       <c r="JN29" s="4"/>
     </row>
     <row r="30" spans="1:274" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="161"/>
+      <c r="A30" s="166"/>
       <c r="B30" s="102"/>
       <c r="C30" s="103"/>
       <c r="D30" s="104"/>
@@ -11717,9 +11843,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11750,10 +11876,10 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="172">
+      <c r="B4" s="177">
         <v>2018.12</v>
       </c>
-      <c r="C4" s="173"/>
+      <c r="C4" s="178"/>
       <c r="D4" s="139">
         <f>SUM(D5:D13)</f>
         <v>42</v>
@@ -11761,7 +11887,7 @@
       <c r="E4" s="140"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="176">
+      <c r="B5" s="181">
         <v>12</v>
       </c>
       <c r="C5" s="143">
@@ -11775,7 +11901,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="177"/>
+      <c r="B6" s="182"/>
       <c r="C6" s="141">
         <v>17</v>
       </c>
@@ -11787,7 +11913,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="177"/>
+      <c r="B7" s="182"/>
       <c r="C7" s="141">
         <v>19</v>
       </c>
@@ -11799,7 +11925,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="177"/>
+      <c r="B8" s="182"/>
       <c r="C8" s="134">
         <v>22</v>
       </c>
@@ -11811,7 +11937,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="177"/>
+      <c r="B9" s="182"/>
       <c r="C9" s="134">
         <v>23</v>
       </c>
@@ -11823,7 +11949,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="177"/>
+      <c r="B10" s="182"/>
       <c r="C10" s="134">
         <v>25</v>
       </c>
@@ -11835,7 +11961,7 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="177"/>
+      <c r="B11" s="182"/>
       <c r="C11" s="134">
         <v>26</v>
       </c>
@@ -11847,7 +11973,7 @@
       </c>
     </row>
     <row r="12" spans="2:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="B12" s="177"/>
+      <c r="B12" s="182"/>
       <c r="C12" s="134">
         <v>29</v>
       </c>
@@ -11859,7 +11985,7 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="178"/>
+      <c r="B13" s="183"/>
       <c r="C13" s="137">
         <v>30</v>
       </c>
@@ -11871,10 +11997,10 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="174">
+      <c r="B14" s="179">
         <v>2019.01</v>
       </c>
-      <c r="C14" s="175"/>
+      <c r="C14" s="180"/>
       <c r="D14" s="154">
         <f>SUM(D15:D23)</f>
         <v>34</v>
@@ -11882,7 +12008,7 @@
       <c r="E14" s="155"/>
     </row>
     <row r="15" spans="2:5" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B15" s="133">
+      <c r="B15" s="184">
         <v>1</v>
       </c>
       <c r="C15" s="134">
@@ -11896,9 +12022,7 @@
       </c>
     </row>
     <row r="16" spans="2:5" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B16" s="133">
-        <v>1</v>
-      </c>
+      <c r="B16" s="185"/>
       <c r="C16" s="134">
         <v>5</v>
       </c>
@@ -11910,9 +12034,7 @@
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="133">
-        <v>1</v>
-      </c>
+      <c r="B17" s="185"/>
       <c r="C17" s="134">
         <v>13</v>
       </c>
@@ -11924,9 +12046,7 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="133">
-        <v>1</v>
-      </c>
+      <c r="B18" s="185"/>
       <c r="C18" s="134">
         <v>15</v>
       </c>
@@ -11938,9 +12058,7 @@
       </c>
     </row>
     <row r="19" spans="2:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="B19" s="133">
-        <v>1</v>
-      </c>
+      <c r="B19" s="185"/>
       <c r="C19" s="134">
         <v>17</v>
       </c>
@@ -11952,9 +12070,7 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="133">
-        <v>1</v>
-      </c>
+      <c r="B20" s="185"/>
       <c r="C20" s="134">
         <v>18</v>
       </c>
@@ -11966,9 +12082,7 @@
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="133">
-        <v>1</v>
-      </c>
+      <c r="B21" s="185"/>
       <c r="C21" s="134">
         <v>21</v>
       </c>
@@ -11980,9 +12094,7 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="133">
-        <v>1</v>
-      </c>
+      <c r="B22" s="185"/>
       <c r="C22" s="134">
         <v>22</v>
       </c>
@@ -11994,9 +12106,7 @@
       </c>
     </row>
     <row r="23" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="136">
-        <v>1</v>
-      </c>
+      <c r="B23" s="186"/>
       <c r="C23" s="137">
         <v>28</v>
       </c>
@@ -12008,10 +12118,10 @@
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="172">
+      <c r="B24" s="177">
         <v>2019.02</v>
       </c>
-      <c r="C24" s="173"/>
+      <c r="C24" s="178"/>
       <c r="D24" s="139">
         <f>SUM(D25:D30)</f>
         <v>20</v>
@@ -12019,7 +12129,7 @@
       <c r="E24" s="142"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="133">
+      <c r="B25" s="184">
         <v>2</v>
       </c>
       <c r="C25" s="134">
@@ -12033,7 +12143,7 @@
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="133"/>
+      <c r="B26" s="185"/>
       <c r="C26" s="134">
         <v>11</v>
       </c>
@@ -12045,7 +12155,7 @@
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="133"/>
+      <c r="B27" s="185"/>
       <c r="C27" s="134">
         <v>12</v>
       </c>
@@ -12057,7 +12167,7 @@
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="133"/>
+      <c r="B28" s="185"/>
       <c r="C28" s="134">
         <v>12</v>
       </c>
@@ -12069,7 +12179,7 @@
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="133"/>
+      <c r="B29" s="185"/>
       <c r="C29" s="134">
         <v>24</v>
       </c>
@@ -12081,7 +12191,7 @@
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="133"/>
+      <c r="B30" s="187"/>
       <c r="C30" s="134">
         <v>26</v>
       </c>
@@ -12089,22 +12199,24 @@
         <v>5</v>
       </c>
       <c r="E30" s="142" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="172">
-        <v>2019.02</v>
-      </c>
-      <c r="C31" s="173"/>
+      <c r="B31" s="177">
+        <v>2019.03</v>
+      </c>
+      <c r="C31" s="178"/>
       <c r="D31" s="139">
-        <f>SUM(D32:D70)</f>
-        <v>30</v>
+        <f>SUM(D32:D43)</f>
+        <v>51</v>
       </c>
       <c r="E31" s="142"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="133"/>
+      <c r="B32" s="133">
+        <v>3</v>
+      </c>
       <c r="C32" s="134">
         <v>2</v>
       </c>
@@ -12112,7 +12224,7 @@
         <v>3</v>
       </c>
       <c r="E32" s="142" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.3">
@@ -12122,7 +12234,7 @@
         <v>6</v>
       </c>
       <c r="E33" s="142" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.3">
@@ -12134,7 +12246,7 @@
         <v>4</v>
       </c>
       <c r="E34" s="142" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.3">
@@ -12146,7 +12258,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="142" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.3">
@@ -12158,7 +12270,7 @@
         <v>3</v>
       </c>
       <c r="E36" s="142" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.3">
@@ -12170,7 +12282,7 @@
         <v>8</v>
       </c>
       <c r="E37" s="142" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.3">
@@ -12182,80 +12294,151 @@
         <v>5</v>
       </c>
       <c r="E38" s="142" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="133"/>
-      <c r="C39" s="134"/>
-      <c r="D39" s="135"/>
-      <c r="E39" s="142"/>
+      <c r="C39" s="134">
+        <v>17</v>
+      </c>
+      <c r="D39" s="135">
+        <v>8</v>
+      </c>
+      <c r="E39" s="142" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="133"/>
-      <c r="C40" s="134"/>
-      <c r="D40" s="135"/>
-      <c r="E40" s="142"/>
+      <c r="C40" s="134">
+        <v>18</v>
+      </c>
+      <c r="D40" s="135">
+        <v>4</v>
+      </c>
+      <c r="E40" s="142" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="133"/>
-      <c r="C41" s="134"/>
-      <c r="D41" s="135"/>
-      <c r="E41" s="142"/>
+      <c r="C41" s="134">
+        <v>26</v>
+      </c>
+      <c r="D41" s="135">
+        <v>4</v>
+      </c>
+      <c r="E41" s="142" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="133"/>
-      <c r="C42" s="134"/>
-      <c r="D42" s="135"/>
-      <c r="E42" s="142"/>
+      <c r="C42" s="134">
+        <v>27</v>
+      </c>
+      <c r="D42" s="135">
+        <v>2</v>
+      </c>
+      <c r="E42" s="142" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="133"/>
-      <c r="C43" s="134"/>
-      <c r="D43" s="135"/>
-      <c r="E43" s="142"/>
+      <c r="C43" s="134">
+        <v>29</v>
+      </c>
+      <c r="D43" s="135">
+        <v>3</v>
+      </c>
+      <c r="E43" s="142" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B44" s="133"/>
-      <c r="C44" s="134"/>
-      <c r="D44" s="135"/>
+      <c r="B44" s="177">
+        <v>2019.04</v>
+      </c>
+      <c r="C44" s="178"/>
+      <c r="D44" s="139">
+        <f>SUM(D45:D56)</f>
+        <v>20</v>
+      </c>
       <c r="E44" s="142"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B45" s="133"/>
-      <c r="C45" s="134"/>
-      <c r="D45" s="135"/>
-      <c r="E45" s="142"/>
+      <c r="C45" s="134">
+        <v>1</v>
+      </c>
+      <c r="D45" s="135">
+        <v>3</v>
+      </c>
+      <c r="E45" s="142" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="133"/>
-      <c r="C46" s="134"/>
-      <c r="D46" s="135"/>
-      <c r="E46" s="142"/>
+      <c r="C46" s="134">
+        <v>3</v>
+      </c>
+      <c r="D46" s="135">
+        <v>3</v>
+      </c>
+      <c r="E46" s="142" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="133"/>
-      <c r="C47" s="134"/>
-      <c r="D47" s="135"/>
-      <c r="E47" s="142"/>
+      <c r="C47" s="134">
+        <v>4</v>
+      </c>
+      <c r="D47" s="135">
+        <v>4</v>
+      </c>
+      <c r="E47" s="142" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="133"/>
-      <c r="C48" s="134"/>
-      <c r="D48" s="135"/>
-      <c r="E48" s="142"/>
+      <c r="C48" s="134">
+        <v>9</v>
+      </c>
+      <c r="D48" s="135">
+        <v>2</v>
+      </c>
+      <c r="E48" s="142" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="133"/>
-      <c r="C49" s="134"/>
-      <c r="D49" s="135"/>
-      <c r="E49" s="142"/>
+      <c r="C49" s="134">
+        <v>10</v>
+      </c>
+      <c r="D49" s="135">
+        <v>4</v>
+      </c>
+      <c r="E49" s="142" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="133"/>
-      <c r="C50" s="134"/>
-      <c r="D50" s="135"/>
-      <c r="E50" s="142"/>
+      <c r="C50" s="134">
+        <v>11</v>
+      </c>
+      <c r="D50" s="135">
+        <v>4</v>
+      </c>
+      <c r="E50" s="142" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" s="133"/>
@@ -12300,12 +12483,15 @@
       <c r="E57" s="130"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="B44:C44"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B5:B13"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B15:B23"/>
+    <mergeCell ref="B25:B30"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Pipette] V4.0 SMT issue
</commit_message>
<xml_diff>
--- a/Plasma Project schedule V1.0.xlsx
+++ b/Plasma Project schedule V1.0.xlsx
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="103">
   <si>
     <t>Femto Project 일정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -534,12 +534,16 @@
     <t>RF Gen CPU PCB 회로 설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Pipette V4.0 SMT issue debugging</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -653,6 +657,15 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -1415,7 +1428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1736,6 +1749,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1779,7 +1795,7 @@
         <xdr:cNvPr id="52" name="직선 화살표 연결선 51">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000034000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1836,7 +1852,7 @@
         <xdr:cNvPr id="15" name="직선 화살표 연결선 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1893,7 +1909,7 @@
         <xdr:cNvPr id="18" name="직선 화살표 연결선 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B9B7B3B-4B32-4051-898C-EE6F25736D05}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B9B7B3B-4B32-4051-898C-EE6F25736D05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1950,7 +1966,7 @@
         <xdr:cNvPr id="21" name="직선 화살표 연결선 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CEEB29C9-2143-40DD-9242-A82E285F4B2E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEEB29C9-2143-40DD-9242-A82E285F4B2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2007,7 +2023,7 @@
         <xdr:cNvPr id="25" name="직선 화살표 연결선 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2375196F-31DF-4BFC-AC62-19AF714F443A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2375196F-31DF-4BFC-AC62-19AF714F443A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2064,7 +2080,7 @@
         <xdr:cNvPr id="28" name="직선 화살표 연결선 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3D1266C4-6D7E-4F8B-8103-59BF7C6FE4FB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D1266C4-6D7E-4F8B-8103-59BF7C6FE4FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2121,7 +2137,7 @@
         <xdr:cNvPr id="32" name="직선 화살표 연결선 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{666CF52C-5D68-4474-8BDD-79976E036787}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{666CF52C-5D68-4474-8BDD-79976E036787}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2178,7 +2194,7 @@
         <xdr:cNvPr id="33" name="직선 화살표 연결선 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{07D67EB1-AD43-42F4-B443-3BB978B9F2AC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07D67EB1-AD43-42F4-B443-3BB978B9F2AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2235,7 +2251,7 @@
         <xdr:cNvPr id="36" name="직선 화살표 연결선 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9A732A08-4D4F-441D-9243-033ACD4A7F32}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A732A08-4D4F-441D-9243-033ACD4A7F32}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2292,7 +2308,7 @@
         <xdr:cNvPr id="38" name="직선 화살표 연결선 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3A864090-2577-47BA-8983-FFA17538A224}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A864090-2577-47BA-8983-FFA17538A224}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2349,7 +2365,7 @@
         <xdr:cNvPr id="41" name="직선 화살표 연결선 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B9CC53C-2611-4F5F-B122-A3165CFAFB90}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B9CC53C-2611-4F5F-B122-A3165CFAFB90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2406,7 +2422,7 @@
         <xdr:cNvPr id="46" name="직선 화살표 연결선 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A6CC6FD7-49CF-4859-9978-820DB474FDCC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6CC6FD7-49CF-4859-9978-820DB474FDCC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2463,7 +2479,7 @@
         <xdr:cNvPr id="14" name="직선 화살표 연결선 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A5A7DBF8-E685-466C-85D3-36D1828C9CBD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5A7DBF8-E685-466C-85D3-36D1828C9CBD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2520,7 +2536,7 @@
         <xdr:cNvPr id="16" name="직선 화살표 연결선 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8D724AD7-DEC3-4BAD-A0BE-EBB685097DA0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D724AD7-DEC3-4BAD-A0BE-EBB685097DA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2577,7 +2593,7 @@
         <xdr:cNvPr id="19" name="직선 화살표 연결선 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E49A8F08-60DF-418D-8D92-E435C42894A7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E49A8F08-60DF-418D-8D92-E435C42894A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2634,7 +2650,7 @@
         <xdr:cNvPr id="17" name="직선 화살표 연결선 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B9B7B3B-4B32-4051-898C-EE6F25736D05}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B9B7B3B-4B32-4051-898C-EE6F25736D05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2691,7 +2707,7 @@
         <xdr:cNvPr id="20" name="직선 화살표 연결선 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CEEB29C9-2143-40DD-9242-A82E285F4B2E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEEB29C9-2143-40DD-9242-A82E285F4B2E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11918,7 +11934,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
+      <selection pane="bottomLeft" activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11930,7 +11946,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="194" t="s">
         <v>23</v>
       </c>
     </row>
@@ -12616,7 +12632,7 @@
       <c r="C59" s="185"/>
       <c r="D59" s="139">
         <f>SUM(D60:D88)</f>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E59" s="142"/>
     </row>
@@ -12682,15 +12698,27 @@
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B65" s="164"/>
-      <c r="C65" s="165"/>
-      <c r="D65" s="166"/>
-      <c r="E65" s="168"/>
+      <c r="C65" s="165">
+        <v>9</v>
+      </c>
+      <c r="D65" s="166">
+        <v>2</v>
+      </c>
+      <c r="E65" s="168" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B66" s="164"/>
-      <c r="C66" s="165"/>
-      <c r="D66" s="166"/>
-      <c r="E66" s="168"/>
+      <c r="C66" s="165">
+        <v>9</v>
+      </c>
+      <c r="D66" s="166">
+        <v>3</v>
+      </c>
+      <c r="E66" s="142" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67" s="164"/>

</xml_diff>